<commit_message>
Dyn Jacobian Matrix Joint Implementation
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29D78E8-29B5-4858-99AC-CE1FB5BB12CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6CA8E2-5BD7-4C04-8B29-969FEEA4E6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
     <sheet name="Bodies" sheetId="1" r:id="rId2"/>
     <sheet name="Joints" sheetId="2" r:id="rId3"/>
     <sheet name="Joints_Drivers" sheetId="5" r:id="rId4"/>
+    <sheet name="Force_Elements" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="95">
   <si>
     <t>Mass</t>
   </si>
@@ -310,6 +311,15 @@
   </si>
   <si>
     <t>Kin</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Torsional Spring</t>
+  </si>
+  <si>
+    <t>Damper</t>
   </si>
 </sst>
 </file>
@@ -501,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -586,6 +596,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,6 +617,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,27 +639,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -668,6 +681,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1054,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B2:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,18 +1090,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="39"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="33">
         <v>2</v>
       </c>
@@ -1088,10 +1110,10 @@
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="33">
         <v>0.5</v>
       </c>
@@ -1101,10 +1123,10 @@
       <c r="S4" s="14"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="37"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="33" t="s">
         <v>91</v>
       </c>
@@ -1141,7 +1163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH197"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB27" sqref="AB26:AB27"/>
     </sheetView>
   </sheetViews>
@@ -1160,110 +1182,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="43" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43" t="s">
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43" t="s">
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="45" t="s">
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="47"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="44"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="42" t="s">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42" t="s">
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42" t="s">
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="43" t="s">
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43" t="s">
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="44" t="s">
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="41" t="s">
+      <c r="S2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="T2" s="42" t="s">
+      <c r="T2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-      <c r="W2" s="43" t="s">
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="41"/>
       <c r="Z2" s="31" t="s">
         <v>69</v>
       </c>
       <c r="AA2" s="31"/>
       <c r="AB2" s="31"/>
-      <c r="AC2" s="43" t="s">
+      <c r="AC2" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="43"/>
-      <c r="AF2" s="43" t="s">
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="AG2" s="43"/>
-      <c r="AH2" s="43"/>
+      <c r="AG2" s="41"/>
+      <c r="AH2" s="41"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1317,8 +1339,8 @@
       <c r="Q3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="44"/>
-      <c r="S3" s="41"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="46"/>
       <c r="T3" s="18" t="s">
         <v>81</v>
       </c>
@@ -4587,6 +4609,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C1:E1"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AC2:AE2"/>
     <mergeCell ref="AF2:AH2"/>
@@ -4603,7 +4626,6 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
-    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4615,7 +4637,7 @@
   <dimension ref="A1:X58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4822,16 +4844,16 @@
       </c>
       <c r="G7" s="50"/>
       <c r="H7" s="50"/>
-      <c r="I7" s="48" t="s">
+      <c r="I7" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48" t="s">
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -4955,11 +4977,11 @@
       </c>
       <c r="G11" s="50"/>
       <c r="H11" s="50"/>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5079,11 +5101,11 @@
       </c>
       <c r="G16" s="50"/>
       <c r="H16" s="50"/>
-      <c r="I16" s="48" t="s">
+      <c r="I16" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
@@ -5162,11 +5184,11 @@
       </c>
       <c r="G20" s="50"/>
       <c r="H20" s="50"/>
-      <c r="I20" s="48" t="s">
+      <c r="I20" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
     </row>
     <row r="21" spans="1:24" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
@@ -5235,16 +5257,16 @@
       <c r="E24" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="51" t="s">
+      <c r="F24" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="G24" s="52"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="51" t="s">
+      <c r="G24" s="53"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="J24" s="52"/>
-      <c r="K24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="54"/>
     </row>
     <row r="25" spans="1:24" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I25" s="10"/>
@@ -5411,15 +5433,15 @@
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="54" t="s">
+      <c r="A35" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="56"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="57"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="10"/>
@@ -5439,11 +5461,11 @@
       <c r="D36" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="48" t="s">
+      <c r="E36" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="10"/>
@@ -5566,18 +5588,6 @@
     <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="F20:H20"/>
@@ -5588,6 +5598,18 @@
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
     <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -5609,7 +5631,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5623,18 +5645,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
@@ -5652,11 +5674,11 @@
       <c r="E2" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="60"/>
       <c r="I2" s="28" t="s">
         <v>62</v>
       </c>
@@ -5712,4 +5734,162 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1356001A-570B-4774-AE32-331534C6A696}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+    </row>
+    <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="57"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+    </row>
+    <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="57"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Forces Processing (Excel and Function)
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6CA8E2-5BD7-4C04-8B29-969FEEA4E6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFE1944-872B-4ED6-9E26-3829E52EA875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Force_Elements" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="98">
   <si>
     <t>Mass</t>
   </si>
@@ -320,6 +321,15 @@
   </si>
   <si>
     <t>Damper</t>
+  </si>
+  <si>
+    <t>Spring Stiffness [N/mm]</t>
+  </si>
+  <si>
+    <t>Damping Coefficient</t>
+  </si>
+  <si>
+    <t>Torsional Constant [Nmm/rad]</t>
   </si>
 </sst>
 </file>
@@ -420,7 +430,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -507,11 +517,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -599,6 +629,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -641,13 +679,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -683,13 +721,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1090,18 +1125,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="40"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="33">
         <v>2</v>
       </c>
@@ -1110,10 +1145,10 @@
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="38"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="33">
         <v>0.5</v>
       </c>
@@ -1123,10 +1158,10 @@
       <c r="S4" s="14"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="33" t="s">
         <v>91</v>
       </c>
@@ -1182,110 +1217,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="41" t="s">
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41" t="s">
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41" t="s">
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="42" t="s">
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="43"/>
-      <c r="AH1" s="44"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="48"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="47" t="s">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47" t="s">
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47" t="s">
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="41" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41" t="s">
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="48" t="s">
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="46" t="s">
+      <c r="S2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="T2" s="47" t="s">
+      <c r="T2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="41" t="s">
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
       <c r="Z2" s="31" t="s">
         <v>69</v>
       </c>
       <c r="AA2" s="31"/>
       <c r="AB2" s="31"/>
-      <c r="AC2" s="41" t="s">
+      <c r="AC2" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="AD2" s="41"/>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41" t="s">
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="AG2" s="41"/>
-      <c r="AH2" s="41"/>
+      <c r="AG2" s="45"/>
+      <c r="AH2" s="45"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1339,8 +1374,8 @@
       <c r="Q3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="48"/>
-      <c r="S3" s="46"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="50"/>
       <c r="T3" s="18" t="s">
         <v>81</v>
       </c>
@@ -4609,11 +4644,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="S1:AH1"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -4626,6 +4656,11 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="S1:AH1"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4657,16 +4692,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -4697,11 +4732,11 @@
       <c r="E2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4799,22 +4834,22 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
@@ -4839,21 +4874,21 @@
       <c r="E7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="51" t="s">
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51" t="s">
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -4935,19 +4970,19 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -4972,16 +5007,16 @@
       <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="51" t="s">
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5059,19 +5094,19 @@
       <c r="X14" s="10"/>
     </row>
     <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
@@ -5096,16 +5131,16 @@
       <c r="E16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="50" t="s">
+      <c r="F16" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="51" t="s">
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
@@ -5142,19 +5177,19 @@
       <c r="X18" s="10"/>
     </row>
     <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -5179,16 +5214,16 @@
       <c r="E20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51" t="s">
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
     </row>
     <row r="21" spans="1:24" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
@@ -5227,19 +5262,19 @@
     </row>
     <row r="22" spans="1:24" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
     </row>
     <row r="24" spans="1:24" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
@@ -5257,16 +5292,16 @@
       <c r="E24" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="52" t="s">
+      <c r="F24" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="G24" s="53"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="52" t="s">
+      <c r="G24" s="57"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="J24" s="53"/>
-      <c r="K24" s="54"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="58"/>
     </row>
     <row r="25" spans="1:24" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I25" s="10"/>
@@ -5275,14 +5310,14 @@
     </row>
     <row r="26" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -5356,12 +5391,12 @@
       <c r="X30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="49"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -5433,15 +5468,15 @@
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="55" t="s">
+      <c r="A35" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="57"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="61"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="10"/>
@@ -5461,11 +5496,11 @@
       <c r="D36" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="51" t="s">
+      <c r="E36" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="10"/>
@@ -5588,6 +5623,18 @@
     <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="F20:H20"/>
@@ -5598,18 +5645,6 @@
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
     <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -5645,18 +5680,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
@@ -5674,11 +5709,11 @@
       <c r="E2" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="60"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="64"/>
       <c r="I2" s="28" t="s">
         <v>62</v>
       </c>
@@ -5741,7 +5776,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5749,25 +5784,26 @@
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="9" max="9" width="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
@@ -5785,17 +5821,19 @@
       <c r="E2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
@@ -5806,24 +5844,25 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
     </row>
     <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="57"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
@@ -5841,23 +5880,27 @@
       <c r="E8" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="30" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="57"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
@@ -5875,20 +5918,23 @@
       <c r="E14" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="50" t="s">
+      <c r="F14" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="30" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="F8:H8"/>
-    <mergeCell ref="A13:H13"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pré Jacobian Eq Changes
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC339D9-671C-40E9-AB2C-CA4080A3E058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805A9F35-0AF1-461B-B5DA-1F5E0BFD8364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9165" yWindow="11385" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2745" yWindow="2955" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -331,9 +331,6 @@
     <t>Crank</t>
   </si>
   <si>
-    <t>Connecting Rode</t>
-  </si>
-  <si>
     <t>Rot Ang [Rad]</t>
   </si>
   <si>
@@ -347,6 +344,9 @@
   </si>
   <si>
     <t>Pure Body Torques [Nmm]</t>
+  </si>
+  <si>
+    <t>Connecting Rod</t>
   </si>
 </sst>
 </file>
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC7" sqref="AC7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,7 +1301,7 @@
       <c r="P2" s="47"/>
       <c r="Q2" s="47"/>
       <c r="R2" s="54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S2" s="52" t="s">
         <v>0</v>
@@ -1312,22 +1312,22 @@
       <c r="U2" s="53"/>
       <c r="V2" s="53"/>
       <c r="W2" s="47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X2" s="47"/>
       <c r="Y2" s="47"/>
       <c r="Z2" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AA2" s="49"/>
       <c r="AB2" s="50"/>
       <c r="AC2" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AD2" s="47"/>
       <c r="AE2" s="47"/>
       <c r="AF2" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AG2" s="47"/>
       <c r="AH2" s="47"/>
@@ -1570,7 +1570,7 @@
         <v>86.6</v>
       </c>
       <c r="D5" s="17">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E5" s="24">
         <v>0</v>
@@ -1612,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="R5" s="40">
-        <v>0.52359999999999995</v>
+        <v>-0.52359999999999995</v>
       </c>
       <c r="S5" s="17">
         <v>0.33600000000000002</v>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="AH5" s="40">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI5" s="40">
         <v>0</v>
@@ -1677,13 +1677,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C6" s="18">
         <v>418.1</v>
       </c>
       <c r="D6" s="17">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E6" s="24">
         <v>0</v>
@@ -1725,16 +1725,18 @@
         <v>1</v>
       </c>
       <c r="R6" s="40">
-        <v>-0.20100000000000001</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="S6" s="17">
         <v>5.25</v>
       </c>
       <c r="T6" s="17">
-        <v>128107</v>
+        <f>1.2810726*10^5</f>
+        <v>128107.26</v>
       </c>
       <c r="U6" s="17">
-        <v>127307</v>
+        <f>1.27307*10^5</f>
+        <v>127306.99999999999</v>
       </c>
       <c r="V6" s="17">
         <v>1345.91</v>
@@ -1871,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="AC7" s="40">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="40">
         <v>0</v>
@@ -1889,13 +1891,13 @@
         <v>0</v>
       </c>
       <c r="AI7" s="40">
-        <v>780</v>
+        <v>0</v>
       </c>
       <c r="AJ7" s="40">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="40">
-        <v>-20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Inertia + Jacobian Debug
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805A9F35-0AF1-461B-B5DA-1F5E0BFD8364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09E8E6E-7CA3-4DE2-8673-50CA959E8564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="2955" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -531,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -637,6 +637,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -655,8 +658,20 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -667,25 +682,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1119,18 +1122,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="46"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="30">
         <v>2</v>
       </c>
@@ -1139,10 +1142,10 @@
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="41"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="30">
         <v>0.5</v>
       </c>
@@ -1152,10 +1155,10 @@
       <c r="S4" s="13"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="30" t="s">
         <v>93</v>
       </c>
@@ -1165,10 +1168,10 @@
       <c r="S5" s="13"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="30"/>
       <c r="E6" s="30" t="s">
         <v>90</v>
@@ -1176,10 +1179,10 @@
       <c r="S6" s="13"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="41"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="30"/>
       <c r="E7" s="39" t="s">
         <v>94</v>
@@ -1204,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,118 +1227,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="51"/>
-      <c r="B1" s="51"/>
-      <c r="C1" s="47" t="s">
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47" t="s">
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47" t="s">
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47" t="s">
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47" t="s">
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="47"/>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="47"/>
-      <c r="AK1" s="47"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="53" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53" t="s">
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="47" t="s">
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47" t="s">
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="54" t="s">
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="S2" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="53" t="s">
+      <c r="S2" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="47" t="s">
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="48" t="s">
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="50"/>
-      <c r="AC2" s="47" t="s">
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="47"/>
-      <c r="AE2" s="47"/>
-      <c r="AF2" s="47" t="s">
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51"/>
+      <c r="AF2" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="AG2" s="47"/>
-      <c r="AH2" s="47"/>
-      <c r="AI2" s="47" t="s">
+      <c r="AG2" s="51"/>
+      <c r="AH2" s="51"/>
+      <c r="AI2" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="AJ2" s="47"/>
-      <c r="AK2" s="47"/>
+      <c r="AJ2" s="51"/>
+      <c r="AK2" s="51"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
@@ -1389,8 +1392,8 @@
       <c r="Q3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="54"/>
-      <c r="S3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="49"/>
       <c r="T3" s="17" t="s">
         <v>69</v>
       </c>
@@ -1615,16 +1618,16 @@
         <v>-0.52359999999999995</v>
       </c>
       <c r="S5" s="17">
-        <v>0.33600000000000002</v>
+        <v>0.33610000000000001</v>
       </c>
       <c r="T5" s="17">
-        <v>1312.93</v>
+        <v>13.79</v>
       </c>
       <c r="U5" s="17">
         <v>1304.74</v>
       </c>
       <c r="V5" s="17">
-        <v>13.79</v>
+        <v>1312.9336000000001</v>
       </c>
       <c r="W5" s="40">
         <v>0</v>
@@ -1645,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="AC5" s="40">
-        <v>0</v>
+        <v>-10000</v>
       </c>
       <c r="AD5" s="40">
         <v>0</v>
@@ -1660,13 +1663,13 @@
         <v>0</v>
       </c>
       <c r="AH5" s="40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AI5" s="40">
-        <v>0</v>
+        <v>173.2</v>
       </c>
       <c r="AJ5" s="40">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="AK5" s="40">
         <v>0</v>
@@ -1728,18 +1731,18 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="S6" s="17">
-        <v>5.25</v>
+        <v>5.2492999999999999</v>
       </c>
       <c r="T6" s="17">
-        <f>1.2810726*10^5</f>
-        <v>128107.26</v>
+        <v>1345.9128000000001</v>
       </c>
       <c r="U6" s="17">
         <f>1.27307*10^5</f>
         <v>127306.99999999999</v>
       </c>
-      <c r="V6" s="17">
-        <v>1345.91</v>
+      <c r="V6" s="41">
+        <f>1.2810726*10^5</f>
+        <v>128107.26</v>
       </c>
       <c r="W6" s="40">
         <v>0</v>
@@ -1843,16 +1846,16 @@
         <v>0</v>
       </c>
       <c r="S7" s="17">
-        <v>3</v>
+        <v>2.9956</v>
       </c>
       <c r="T7" s="17">
-        <v>5192.3500000000004</v>
+        <v>1997.056</v>
       </c>
       <c r="U7" s="17">
         <v>3994.1</v>
       </c>
       <c r="V7" s="17">
-        <v>1997.1</v>
+        <v>5192.3455999999996</v>
       </c>
       <c r="W7" s="40">
         <v>0</v>
@@ -2407,9 +2410,6 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -2425,7 +2425,6 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -4978,6 +4977,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -4991,12 +4996,6 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5008,7 +5007,7 @@
   <dimension ref="A1:X58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5107,7 +5106,7 @@
         <v>173.2</v>
       </c>
       <c r="G3" s="4">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="H3" s="4">
         <v>0</v>
@@ -5215,16 +5214,16 @@
       </c>
       <c r="G7" s="57"/>
       <c r="H7" s="57"/>
-      <c r="I7" s="55" t="s">
+      <c r="I7" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55" t="s">
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -5348,11 +5347,11 @@
       </c>
       <c r="G11" s="57"/>
       <c r="H11" s="57"/>
-      <c r="I11" s="55" t="s">
+      <c r="I11" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5472,11 +5471,11 @@
       </c>
       <c r="G16" s="57"/>
       <c r="H16" s="57"/>
-      <c r="I16" s="55" t="s">
+      <c r="I16" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
@@ -5555,11 +5554,11 @@
       </c>
       <c r="G20" s="57"/>
       <c r="H20" s="57"/>
-      <c r="I20" s="55" t="s">
+      <c r="I20" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
     </row>
     <row r="21" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
@@ -5628,16 +5627,16 @@
       <c r="E24" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="58" t="s">
+      <c r="F24" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="59"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="58" t="s">
+      <c r="G24" s="60"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="J24" s="59"/>
-      <c r="K24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="61"/>
     </row>
     <row r="25" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I25" s="10"/>
@@ -5804,15 +5803,15 @@
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="61" t="s">
+      <c r="A35" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="62"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="63"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="64"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="10"/>
@@ -5832,11 +5831,11 @@
       <c r="D36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="55" t="s">
+      <c r="E36" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="10"/>
@@ -5884,7 +5883,8 @@
         <v>173.2</v>
       </c>
       <c r="F38" s="14">
-        <v>100</v>
+        <f>-100</f>
+        <v>-100</v>
       </c>
       <c r="G38" s="14">
         <v>0</v>
@@ -5959,18 +5959,6 @@
     <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="F20:H20"/>
@@ -5981,6 +5969,18 @@
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
     <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -6016,18 +6016,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -6045,11 +6045,11 @@
       <c r="E2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="67"/>
       <c r="I2" s="26" t="s">
         <v>56</v>
       </c>
@@ -6207,24 +6207,24 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="62"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="62"/>
-      <c r="O11" s="62"/>
-      <c r="P11" s="63"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="64"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
@@ -6250,16 +6250,16 @@
       <c r="I12" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="J12" s="47" t="s">
+      <c r="J12" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47" t="s">
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
       <c r="P12" s="37" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Final Dynamics MMKS and MKS working
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09E8E6E-7CA3-4DE2-8673-50CA959E8564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D72A94-5904-4EB6-A4C0-6C57AB44B8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -658,6 +658,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -668,27 +680,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1109,7 +1109,7 @@
   <dimension ref="B2:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,118 +1227,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="51" t="s">
+      <c r="A1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51" t="s">
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51" t="s">
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51" t="s">
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="48"/>
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="48"/>
+      <c r="AI1" s="48"/>
+      <c r="AJ1" s="48"/>
+      <c r="AK1" s="48"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="50" t="s">
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50" t="s">
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="51" t="s">
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51" t="s">
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="52" t="s">
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="S2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="50" t="s">
+      <c r="S2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="51" t="s">
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="53" t="s">
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="51" t="s">
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
-      <c r="AF2" s="51" t="s">
+      <c r="AD2" s="48"/>
+      <c r="AE2" s="48"/>
+      <c r="AF2" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="AG2" s="51"/>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51" t="s">
+      <c r="AG2" s="48"/>
+      <c r="AH2" s="48"/>
+      <c r="AI2" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
+      <c r="AJ2" s="48"/>
+      <c r="AK2" s="48"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
@@ -1392,8 +1392,8 @@
       <c r="Q3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="52"/>
-      <c r="S3" s="49"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="53"/>
       <c r="T3" s="17" t="s">
         <v>69</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="AC5" s="40">
-        <v>-10000</v>
+        <v>0</v>
       </c>
       <c r="AD5" s="40">
         <v>0</v>
@@ -1663,13 +1663,13 @@
         <v>0</v>
       </c>
       <c r="AH5" s="40">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AI5" s="40">
-        <v>173.2</v>
+        <v>0</v>
       </c>
       <c r="AJ5" s="40">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="AK5" s="40">
         <v>0</v>
@@ -4977,12 +4977,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -4996,6 +4990,12 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5007,7 +5007,7 @@
   <dimension ref="A1:X58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5027,16 +5027,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -5067,11 +5067,11 @@
       <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -5169,22 +5169,22 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
@@ -5209,21 +5209,21 @@
       <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="58" t="s">
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58" t="s">
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -5305,19 +5305,19 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5342,16 +5342,16 @@
       <c r="E11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="57" t="s">
+      <c r="F11" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="58" t="s">
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5429,19 +5429,19 @@
       <c r="X14" s="10"/>
     </row>
     <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
@@ -5466,16 +5466,16 @@
       <c r="E16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="57" t="s">
+      <c r="F16" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="58" t="s">
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
@@ -5512,19 +5512,19 @@
       <c r="X18" s="10"/>
     </row>
     <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -5549,16 +5549,16 @@
       <c r="E20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="57" t="s">
+      <c r="F20" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58" t="s">
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="58"/>
-      <c r="K20" s="58"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="56"/>
     </row>
     <row r="21" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
@@ -5597,19 +5597,19 @@
     </row>
     <row r="22" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
     </row>
     <row r="24" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
@@ -5645,14 +5645,14 @@
     </row>
     <row r="26" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -5726,12 +5726,12 @@
       <c r="X30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -5831,11 +5831,11 @@
       <c r="D36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="58" t="s">
+      <c r="E36" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="10"/>
@@ -5959,6 +5959,18 @@
     <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="F20:H20"/>
@@ -5969,18 +5981,6 @@
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
     <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -6105,17 +6105,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
       <c r="L1" s="32"/>
@@ -6138,11 +6138,11 @@
       <c r="E2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
       <c r="I2" s="28" t="s">
         <v>81</v>
       </c>
@@ -6169,17 +6169,17 @@
       <c r="N3" s="35"/>
     </row>
     <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
@@ -6197,11 +6197,11 @@
       <c r="E7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
       <c r="I7" s="28" t="s">
         <v>82</v>
       </c>
@@ -6242,24 +6242,24 @@
       <c r="E12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="57" t="s">
+      <c r="F12" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
       <c r="I12" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="J12" s="51" t="s">
+      <c r="J12" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51" t="s">
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
       <c r="P12" s="37" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Final MBS Patch Commit
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D72A94-5904-4EB6-A4C0-6C57AB44B8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7071A039-9145-491B-B441-BFA014A40092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11280" yWindow="1620" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="106">
   <si>
     <t>Mass</t>
   </si>
@@ -347,6 +347,12 @@
   </si>
   <si>
     <t>Connecting Rod</t>
+  </si>
+  <si>
+    <t>Units System</t>
+  </si>
+  <si>
+    <t>[SI/MKS or MMKS]</t>
   </si>
 </sst>
 </file>
@@ -658,8 +664,20 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -670,25 +688,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1106,16 +1112,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
-  <dimension ref="B2:S7"/>
+  <dimension ref="B2:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I10:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
     <col min="9" max="9" width="27.85546875" customWidth="1"/>
     <col min="13" max="13" width="31.140625" customWidth="1"/>
     <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
@@ -1189,8 +1195,19 @@
       </c>
       <c r="S7" s="13"/>
     </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="42"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="39" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:C4"/>
@@ -1207,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
@@ -1227,118 +1244,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="48" t="s">
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48" t="s">
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48" t="s">
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48" t="s">
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48" t="s">
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AI1" s="48"/>
-      <c r="AJ1" s="48"/>
-      <c r="AK1" s="48"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="54" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54" t="s">
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="48" t="s">
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48" t="s">
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="55" t="s">
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="S2" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="54" t="s">
+      <c r="S2" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="48" t="s">
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="49" t="s">
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="48" t="s">
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48"/>
-      <c r="AF2" s="48" t="s">
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51"/>
+      <c r="AF2" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="AG2" s="48"/>
-      <c r="AH2" s="48"/>
-      <c r="AI2" s="48" t="s">
+      <c r="AG2" s="51"/>
+      <c r="AH2" s="51"/>
+      <c r="AI2" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
+      <c r="AJ2" s="51"/>
+      <c r="AK2" s="51"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
@@ -1392,8 +1409,8 @@
       <c r="Q3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="55"/>
-      <c r="S3" s="53"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="49"/>
       <c r="T3" s="17" t="s">
         <v>69</v>
       </c>
@@ -4977,6 +4994,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -4990,12 +5013,6 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5027,16 +5044,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -5067,11 +5084,11 @@
       <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -5169,22 +5186,22 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
@@ -5209,21 +5226,21 @@
       <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="56" t="s">
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56" t="s">
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -5305,19 +5322,19 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5342,16 +5359,16 @@
       <c r="E11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="58" t="s">
+      <c r="F11" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="56" t="s">
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5429,19 +5446,19 @@
       <c r="X14" s="10"/>
     </row>
     <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
@@ -5466,16 +5483,16 @@
       <c r="E16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="58" t="s">
+      <c r="F16" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="56" t="s">
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
@@ -5512,19 +5529,19 @@
       <c r="X18" s="10"/>
     </row>
     <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="56"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -5549,16 +5566,16 @@
       <c r="E20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="58" t="s">
+      <c r="F20" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="56" t="s">
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
     </row>
     <row r="21" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
@@ -5597,19 +5614,19 @@
     </row>
     <row r="22" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
     </row>
     <row r="24" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
@@ -5645,14 +5662,14 @@
     </row>
     <row r="26" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -5726,12 +5743,12 @@
       <c r="X30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -5831,11 +5848,11 @@
       <c r="D36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="56" t="s">
+      <c r="E36" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="10"/>
@@ -5959,18 +5976,6 @@
     <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="F20:H20"/>
@@ -5981,6 +5986,18 @@
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
     <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -6105,17 +6122,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
       <c r="L1" s="32"/>
@@ -6138,11 +6155,11 @@
       <c r="E2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
       <c r="I2" s="28" t="s">
         <v>81</v>
       </c>
@@ -6169,17 +6186,17 @@
       <c r="N3" s="35"/>
     </row>
     <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
@@ -6197,11 +6214,11 @@
       <c r="E7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
       <c r="I7" s="28" t="s">
         <v>82</v>
       </c>
@@ -6242,24 +6259,24 @@
       <c r="E12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="58" t="s">
+      <c r="F12" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
       <c r="I12" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="J12" s="48" t="s">
+      <c r="J12" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48" t="s">
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
       <c r="P12" s="37" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Function for Force and Torque Implementation
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7071A039-9145-491B-B441-BFA014A40092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89A1153-FE62-486C-9D7F-7E7648F217A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1620" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11805" yWindow="7515" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="125">
   <si>
     <t>Mass</t>
   </si>
@@ -319,12 +319,6 @@
     <t>Dyn</t>
   </si>
   <si>
-    <t>+g/-g [Nmm]</t>
-  </si>
-  <si>
-    <t>Inertia Moment [kg*mm^-2]</t>
-  </si>
-  <si>
     <t>Bodies ID</t>
   </si>
   <si>
@@ -334,18 +328,6 @@
     <t>Rot Ang [Rad]</t>
   </si>
   <si>
-    <t>Body Forces [N]</t>
-  </si>
-  <si>
-    <t>Initial Translational Vel [mm/s]</t>
-  </si>
-  <si>
-    <t>Initial Rotational Vel [rad/s]</t>
-  </si>
-  <si>
-    <t>Pure Body Torques [Nmm]</t>
-  </si>
-  <si>
     <t>Connecting Rod</t>
   </si>
   <si>
@@ -353,6 +335,81 @@
   </si>
   <si>
     <t>[SI/MKS or MMKS]</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>Body Forces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pure Body Torques </t>
+  </si>
+  <si>
+    <t>Initial Translational Vel</t>
+  </si>
+  <si>
+    <t>Initial Rotational Vel</t>
+  </si>
+  <si>
+    <t>Inertia Moment</t>
+  </si>
+  <si>
+    <t>MKS Unit System</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Rad</t>
+  </si>
+  <si>
+    <t>Inertia</t>
+  </si>
+  <si>
+    <t>kg*mm^-2</t>
+  </si>
+  <si>
+    <t>mmks Unit System</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>kg*m^-2</t>
+  </si>
+  <si>
+    <t>+g/-g</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>m*s^-2</t>
+  </si>
+  <si>
+    <t>mm*s^-2</t>
+  </si>
+  <si>
+    <t>mmks</t>
   </si>
 </sst>
 </file>
@@ -537,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -646,6 +703,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -671,9 +740,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1112,101 +1178,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
-  <dimension ref="B2:S8"/>
+  <dimension ref="B2:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I10:I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="13" max="13" width="31.140625" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="45"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="49"/>
+      <c r="I2" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="45"/>
+      <c r="L2" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" s="45"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="47"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="30">
         <v>2</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>22</v>
       </c>
+      <c r="I3" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="30">
         <v>0.5</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>22</v>
       </c>
+      <c r="I4" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="L4" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="42" t="s">
+        <v>112</v>
+      </c>
       <c r="S4" s="13"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="42"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="30" t="s">
         <v>93</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>78</v>
       </c>
+      <c r="I5" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="J5" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>113</v>
+      </c>
       <c r="S5" s="13"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="30"/>
       <c r="E6" s="30" t="s">
         <v>90</v>
       </c>
+      <c r="I6" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="J6" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="M6" s="42" t="s">
+        <v>22</v>
+      </c>
       <c r="S6" s="13"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="42"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="30"/>
       <c r="E7" s="39" t="s">
-        <v>94</v>
+        <v>120</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="J7" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="L7" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="M7" s="42" t="s">
+        <v>116</v>
       </c>
       <c r="S7" s="13"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="30"/>
+      <c r="B8" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="46"/>
+      <c r="D8" s="30" t="s">
+        <v>124</v>
+      </c>
       <c r="E8" s="39" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="I8" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="J8" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="L8" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="M8" s="42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="I9" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="L9" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="M9" s="43" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L2:M2"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B2:E2"/>
@@ -1224,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI18" sqref="AI18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,125 +1409,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="51" t="s">
+      <c r="A1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51" t="s">
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51" t="s">
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51" t="s">
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="45"/>
+      <c r="AF1" s="45"/>
+      <c r="AG1" s="45"/>
+      <c r="AH1" s="45"/>
+      <c r="AI1" s="45"/>
+      <c r="AJ1" s="45"/>
+      <c r="AK1" s="45"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="50" t="s">
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50" t="s">
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="51" t="s">
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51" t="s">
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="S2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="53" t="s">
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="S2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
-      <c r="AF2" s="51" t="s">
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="AG2" s="51"/>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51" t="s">
+      <c r="AG2" s="45"/>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="45"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>2</v>
@@ -1409,8 +1574,8 @@
       <c r="Q3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="52"/>
-      <c r="S3" s="49"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="53"/>
       <c r="T3" s="17" t="s">
         <v>69</v>
       </c>
@@ -1551,22 +1716,22 @@
       <c r="AB4" s="40">
         <v>0</v>
       </c>
-      <c r="AC4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="40">
+      <c r="AC4" s="44">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="44">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="44">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="44">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="44">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="44">
         <v>0</v>
       </c>
       <c r="AI4" s="40">
@@ -1584,7 +1749,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" s="18">
         <v>86.6</v>
@@ -1664,23 +1829,23 @@
       <c r="AB5" s="40">
         <v>0</v>
       </c>
-      <c r="AC5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="40">
-        <v>5000</v>
+      <c r="AC5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="44">
+        <v>5</v>
       </c>
       <c r="AI5" s="40">
         <v>0</v>
@@ -1697,7 +1862,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C6" s="18">
         <v>418.1</v>
@@ -1779,22 +1944,22 @@
       <c r="AB6" s="40">
         <v>0</v>
       </c>
-      <c r="AC6" s="40">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="40">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="40">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="40">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="40">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="40">
+      <c r="AC6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="44">
         <v>0</v>
       </c>
       <c r="AI6" s="40">
@@ -1892,22 +2057,22 @@
       <c r="AB7" s="40">
         <v>0</v>
       </c>
-      <c r="AC7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="40">
+      <c r="AC7" s="44">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="44">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="44">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="44">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="44">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="44">
         <v>0</v>
       </c>
       <c r="AI7" s="40">
@@ -5024,7 +5189,7 @@
   <dimension ref="A1:X58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5044,16 +5209,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -5084,11 +5249,11 @@
       <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -5186,22 +5351,22 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
@@ -5226,21 +5391,21 @@
       <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="58" t="s">
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58" t="s">
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -5322,19 +5487,19 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5359,16 +5524,16 @@
       <c r="E11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="57" t="s">
+      <c r="F11" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="58" t="s">
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5446,19 +5611,19 @@
       <c r="X14" s="10"/>
     </row>
     <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
@@ -5483,16 +5648,16 @@
       <c r="E16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="57" t="s">
+      <c r="F16" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="58" t="s">
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
@@ -5529,19 +5694,19 @@
       <c r="X18" s="10"/>
     </row>
     <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -5566,16 +5731,16 @@
       <c r="E20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="57" t="s">
+      <c r="F20" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58" t="s">
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="58"/>
-      <c r="K20" s="58"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
     </row>
     <row r="21" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
@@ -5614,19 +5779,19 @@
     </row>
     <row r="22" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
     </row>
     <row r="24" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
@@ -5644,16 +5809,16 @@
       <c r="E24" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="59" t="s">
+      <c r="F24" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="60"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="59" t="s">
+      <c r="G24" s="63"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="J24" s="60"/>
-      <c r="K24" s="61"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="64"/>
     </row>
     <row r="25" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I25" s="10"/>
@@ -5662,14 +5827,14 @@
     </row>
     <row r="26" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -5743,12 +5908,12 @@
       <c r="X30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -5820,15 +5985,15 @@
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="62" t="s">
+      <c r="A35" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="63"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="64"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="66"/>
+      <c r="G35" s="67"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="10"/>
@@ -5848,11 +6013,11 @@
       <c r="D36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="58" t="s">
+      <c r="E36" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="10"/>
@@ -6016,10 +6181,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4658AC4-6667-4045-B0FE-42E281567C35}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6033,18 +6198,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -6062,11 +6227,11 @@
       <c r="E2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="66"/>
-      <c r="H2" s="67"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
       <c r="I2" s="26" t="s">
         <v>56</v>
       </c>
@@ -6088,6 +6253,11 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I4" s="27"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6109,7 +6279,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6122,17 +6292,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
       <c r="L1" s="32"/>
@@ -6155,11 +6325,11 @@
       <c r="E2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
       <c r="I2" s="28" t="s">
         <v>81</v>
       </c>
@@ -6186,17 +6356,17 @@
       <c r="N3" s="35"/>
     </row>
     <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
@@ -6214,34 +6384,34 @@
       <c r="E7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
       <c r="I7" s="28" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="64"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="67"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
@@ -6259,24 +6429,24 @@
       <c r="E12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="57" t="s">
+      <c r="F12" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
       <c r="I12" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="J12" s="51" t="s">
+      <c r="J12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51" t="s">
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
       <c r="P12" s="37" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Final MBS Commit, Before Pos Porcessing
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89A1153-FE62-486C-9D7F-7E7648F217A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01260D7-2243-4D1B-B9EE-774B08D34489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11805" yWindow="7515" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="1185" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="129">
   <si>
     <t>Mass</t>
   </si>
@@ -410,6 +410,18 @@
   </si>
   <si>
     <t>mmks</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Rotational input</t>
+  </si>
+  <si>
+    <t>@(t)0.523-0.3*t</t>
+  </si>
+  <si>
+    <t>Polynomial</t>
   </si>
 </sst>
 </file>
@@ -733,6 +745,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -745,22 +766,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1389,7 +1401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AI18" sqref="AI18"/>
     </sheetView>
   </sheetViews>
@@ -1409,8 +1421,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
       <c r="C1" s="45" t="s">
         <v>30</v>
       </c>
@@ -1458,23 +1470,23 @@
       <c r="AK1" s="45"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="54" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54" t="s">
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
       <c r="L2" s="45" t="s">
         <v>33</v>
       </c>
@@ -1485,27 +1497,27 @@
       </c>
       <c r="P2" s="45"/>
       <c r="Q2" s="45"/>
-      <c r="R2" s="55" t="s">
+      <c r="R2" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="S2" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="54" t="s">
+      <c r="S2" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
       <c r="W2" s="45" t="s">
         <v>103</v>
       </c>
       <c r="X2" s="45"/>
       <c r="Y2" s="45"/>
-      <c r="Z2" s="56" t="s">
+      <c r="Z2" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="58"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="54"/>
       <c r="AC2" s="45" t="s">
         <v>101</v>
       </c>
@@ -1574,8 +1586,8 @@
       <c r="Q3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="55"/>
-      <c r="S3" s="53"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="56"/>
       <c r="T3" s="17" t="s">
         <v>69</v>
       </c>
@@ -5159,12 +5171,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -5178,6 +5184,12 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5209,16 +5221,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -5249,11 +5261,11 @@
       <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -5351,22 +5363,22 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
@@ -5391,21 +5403,21 @@
       <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="61" t="s">
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61" t="s">
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="61"/>
-      <c r="N7" s="61"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -5487,19 +5499,19 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5524,16 +5536,16 @@
       <c r="E11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="60" t="s">
+      <c r="F11" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="61" t="s">
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5611,19 +5623,19 @@
       <c r="X14" s="10"/>
     </row>
     <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
@@ -5648,16 +5660,16 @@
       <c r="E16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="60" t="s">
+      <c r="F16" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="61" t="s">
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
@@ -5694,19 +5706,19 @@
       <c r="X18" s="10"/>
     </row>
     <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -5731,16 +5743,16 @@
       <c r="E20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="60" t="s">
+      <c r="F20" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="61" t="s">
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="59"/>
     </row>
     <row r="21" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
@@ -5779,19 +5791,19 @@
     </row>
     <row r="22" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="59" t="s">
+      <c r="A23" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="59"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
     </row>
     <row r="24" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
@@ -5827,14 +5839,14 @@
     </row>
     <row r="26" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="59" t="s">
+      <c r="A27" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -5908,12 +5920,12 @@
       <c r="X30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="59" t="s">
+      <c r="A31" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -6013,11 +6025,11 @@
       <c r="D36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="61" t="s">
+      <c r="E36" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="10"/>
@@ -6141,6 +6153,18 @@
     <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="F20:H20"/>
@@ -6151,18 +6175,6 @@
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
     <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -6183,8 +6195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4658AC4-6667-4045-B0FE-42E281567C35}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6240,16 +6252,36 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="14"/>
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="14">
+        <v>2</v>
+      </c>
+      <c r="E3" s="14">
+        <v>6</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I4" s="27"/>
@@ -6265,7 +6297,7 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{2127DDA1-6D8E-4B00-8D96-D683E7741146}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{C29CF91F-D32A-47CE-8C1A-1D1B33C14C9E}">
       <formula1>"Spherical,Universal,Revolute,Translation,Cylindrical,Simple,Ground,Driver"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6292,17 +6324,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
       <c r="L1" s="32"/>
@@ -6325,11 +6357,11 @@
       <c r="E2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
       <c r="I2" s="28" t="s">
         <v>81</v>
       </c>
@@ -6356,17 +6388,17 @@
       <c r="N3" s="35"/>
     </row>
     <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
@@ -6384,11 +6416,11 @@
       <c r="E7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
       <c r="I7" s="28" t="s">
         <v>82</v>
       </c>
@@ -6429,11 +6461,11 @@
       <c r="E12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="60" t="s">
+      <c r="F12" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
       <c r="I12" s="28" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
LM working/Non Linear Springs and Dampers
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8321D667-F8D1-43DF-8620-912423C69082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD101A9-DA4A-41F8-8CCD-8E9B426A9487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="1185" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="133">
   <si>
     <t>Mass</t>
   </si>
@@ -280,12 +280,6 @@
     <t>Damper</t>
   </si>
   <si>
-    <t>Spring Stiffness [N/mm]</t>
-  </si>
-  <si>
-    <t>Damping Coefficient</t>
-  </si>
-  <si>
     <t>Torsional Constant [Nmm/rad]</t>
   </si>
   <si>
@@ -410,6 +404,36 @@
   </si>
   <si>
     <t>mmks</t>
+  </si>
+  <si>
+    <t>Linear - Spring Stiffness [N/mm]</t>
+  </si>
+  <si>
+    <t>Linear - Damping Coefficient</t>
+  </si>
+  <si>
+    <t>@(x) Non Linear Force Function (x-Vel)</t>
+  </si>
+  <si>
+    <t>@(x) Non Linear Force Function (x-Displ)</t>
+  </si>
+  <si>
+    <t>Function 1</t>
+  </si>
+  <si>
+    <t>Function 2</t>
+  </si>
+  <si>
+    <t>Function 3</t>
+  </si>
+  <si>
+    <t>1st Interval</t>
+  </si>
+  <si>
+    <t>2nd Interval</t>
+  </si>
+  <si>
+    <t>3rd Interval</t>
   </si>
 </sst>
 </file>
@@ -503,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -590,11 +614,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -677,8 +714,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -688,79 +723,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -772,15 +819,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -795,6 +833,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1180,7 +1248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B2:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1195,177 +1263,177 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="49"/>
-      <c r="I2" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="J2" s="45"/>
-      <c r="L2" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" s="45"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
+      <c r="I2" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" s="44"/>
+      <c r="L2" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="M2" s="44"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="30">
         <v>2</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="J3" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="L3" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="M3" s="42" t="s">
-        <v>111</v>
+      <c r="I3" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="M3" s="38" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="46"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="30">
         <v>0.5</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="L4" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" s="42" t="s">
-        <v>112</v>
+      <c r="I4" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="L4" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="38" t="s">
+        <v>110</v>
       </c>
       <c r="S4" s="13"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="46"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="J5" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="L5" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="M5" s="42" t="s">
-        <v>113</v>
+      <c r="I5" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="L5" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="38" t="s">
+        <v>111</v>
       </c>
       <c r="S5" s="13"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="46"/>
+      <c r="B6" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="45"/>
       <c r="D6" s="30"/>
       <c r="E6" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="J6" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J6" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="M6" s="42" t="s">
+      <c r="L6" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="M6" s="38" t="s">
         <v>22</v>
       </c>
       <c r="S6" s="13"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="46"/>
+      <c r="B7" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="45"/>
       <c r="D7" s="30"/>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="L7" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="M7" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="S7" s="13"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="45"/>
+      <c r="D8" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="L8" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="M8" s="38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="I9" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="J9" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="I7" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="J7" s="42" t="s">
+      <c r="L9" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="L7" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="M7" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="S7" s="13"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="I8" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="J8" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="L8" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="M8" s="42" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I9" s="43" t="s">
+      <c r="M9" s="39" t="s">
         <v>121</v>
-      </c>
-      <c r="J9" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="L9" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="M9" s="43" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AI18" sqref="AI18"/>
     </sheetView>
   </sheetViews>
@@ -1409,125 +1477,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45" t="s">
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45" t="s">
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45" t="s">
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="45"/>
-      <c r="AJ1" s="45"/>
-      <c r="AK1" s="45"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="45" t="s">
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45" t="s">
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="S2" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="54" t="s">
-        <v>105</v>
-      </c>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="45" t="s">
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="56" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="58"/>
-      <c r="AC2" s="45" t="s">
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="AD2" s="45"/>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="45" t="s">
+      <c r="X2" s="44"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ2" s="45"/>
-      <c r="AK2" s="45"/>
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="53"/>
+      <c r="AC2" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
+      <c r="AF2" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG2" s="44"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>2</v>
@@ -1574,8 +1642,8 @@
       <c r="Q3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="55"/>
-      <c r="S3" s="53"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="55"/>
       <c r="T3" s="17" t="s">
         <v>69</v>
       </c>
@@ -1621,13 +1689,13 @@
       <c r="AH3" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="AI3" s="36" t="s">
+      <c r="AI3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="AJ3" s="36" t="s">
+      <c r="AJ3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="AK3" s="36" t="s">
+      <c r="AK3" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1647,43 +1715,43 @@
       <c r="E4" s="17">
         <v>0</v>
       </c>
-      <c r="F4" s="40">
-        <v>0</v>
-      </c>
-      <c r="G4" s="40">
-        <v>0</v>
-      </c>
-      <c r="H4" s="40">
-        <v>0</v>
-      </c>
-      <c r="I4" s="40">
-        <v>0</v>
-      </c>
-      <c r="J4" s="40">
-        <v>0</v>
-      </c>
-      <c r="K4" s="40">
-        <v>0</v>
-      </c>
-      <c r="L4" s="40">
-        <v>0</v>
-      </c>
-      <c r="M4" s="40">
-        <v>0</v>
-      </c>
-      <c r="N4" s="40">
-        <v>0</v>
-      </c>
-      <c r="O4" s="40">
-        <v>0</v>
-      </c>
-      <c r="P4" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="40">
-        <v>0</v>
-      </c>
-      <c r="R4" s="40">
+      <c r="F4" s="36">
+        <v>0</v>
+      </c>
+      <c r="G4" s="36">
+        <v>0</v>
+      </c>
+      <c r="H4" s="36">
+        <v>0</v>
+      </c>
+      <c r="I4" s="36">
+        <v>0</v>
+      </c>
+      <c r="J4" s="36">
+        <v>0</v>
+      </c>
+      <c r="K4" s="36">
+        <v>0</v>
+      </c>
+      <c r="L4" s="36">
+        <v>0</v>
+      </c>
+      <c r="M4" s="36">
+        <v>0</v>
+      </c>
+      <c r="N4" s="36">
+        <v>0</v>
+      </c>
+      <c r="O4" s="36">
+        <v>0</v>
+      </c>
+      <c r="P4" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="36">
+        <v>0</v>
+      </c>
+      <c r="R4" s="36">
         <v>0</v>
       </c>
       <c r="S4" s="17">
@@ -1698,49 +1766,49 @@
       <c r="V4" s="17">
         <v>0</v>
       </c>
-      <c r="W4" s="40">
-        <v>0</v>
-      </c>
-      <c r="X4" s="40">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="40">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="44">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="44">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="44">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="40">
+      <c r="W4" s="36">
+        <v>0</v>
+      </c>
+      <c r="X4" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="36">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="36">
         <v>0</v>
       </c>
     </row>
@@ -1749,7 +1817,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C5" s="18">
         <v>86.6</v>
@@ -1760,43 +1828,43 @@
       <c r="E5" s="24">
         <v>0</v>
       </c>
-      <c r="F5" s="40">
-        <v>0</v>
-      </c>
-      <c r="G5" s="40">
-        <v>0</v>
-      </c>
-      <c r="H5" s="40">
-        <v>0</v>
-      </c>
-      <c r="I5" s="40">
-        <v>0</v>
-      </c>
-      <c r="J5" s="40">
-        <v>0</v>
-      </c>
-      <c r="K5" s="40">
-        <v>0</v>
-      </c>
-      <c r="L5" s="40">
-        <v>0</v>
-      </c>
-      <c r="M5" s="40">
-        <v>0</v>
-      </c>
-      <c r="N5" s="40">
-        <v>0</v>
-      </c>
-      <c r="O5" s="40">
-        <v>0</v>
-      </c>
-      <c r="P5" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="40">
+      <c r="F5" s="36">
+        <v>0</v>
+      </c>
+      <c r="G5" s="36">
+        <v>0</v>
+      </c>
+      <c r="H5" s="36">
+        <v>0</v>
+      </c>
+      <c r="I5" s="36">
+        <v>0</v>
+      </c>
+      <c r="J5" s="36">
+        <v>0</v>
+      </c>
+      <c r="K5" s="36">
+        <v>0</v>
+      </c>
+      <c r="L5" s="36">
+        <v>0</v>
+      </c>
+      <c r="M5" s="36">
+        <v>0</v>
+      </c>
+      <c r="N5" s="36">
+        <v>0</v>
+      </c>
+      <c r="O5" s="36">
+        <v>0</v>
+      </c>
+      <c r="P5" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="36">
         <v>1</v>
       </c>
-      <c r="R5" s="40">
+      <c r="R5" s="36">
         <v>-0.52359999999999995</v>
       </c>
       <c r="S5" s="17">
@@ -1811,49 +1879,49 @@
       <c r="V5" s="17">
         <v>1312.9336000000001</v>
       </c>
-      <c r="W5" s="40">
-        <v>0</v>
-      </c>
-      <c r="X5" s="40">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="40">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="44">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="44">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="44">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="44">
+      <c r="W5" s="36">
+        <v>0</v>
+      </c>
+      <c r="X5" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="36">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="36">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="36">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="40">
         <v>5</v>
       </c>
-      <c r="AI5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="40">
+      <c r="AI5" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="36">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="36">
         <v>0</v>
       </c>
     </row>
@@ -1862,7 +1930,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" s="18">
         <v>418.1</v>
@@ -1873,43 +1941,43 @@
       <c r="E6" s="24">
         <v>0</v>
       </c>
-      <c r="F6" s="40">
-        <v>0</v>
-      </c>
-      <c r="G6" s="40">
-        <v>0</v>
-      </c>
-      <c r="H6" s="40">
-        <v>0</v>
-      </c>
-      <c r="I6" s="40">
-        <v>0</v>
-      </c>
-      <c r="J6" s="40">
-        <v>0</v>
-      </c>
-      <c r="K6" s="40">
-        <v>0</v>
-      </c>
-      <c r="L6" s="40">
-        <v>0</v>
-      </c>
-      <c r="M6" s="40">
-        <v>0</v>
-      </c>
-      <c r="N6" s="40">
-        <v>0</v>
-      </c>
-      <c r="O6" s="40">
-        <v>0</v>
-      </c>
-      <c r="P6" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="40">
+      <c r="F6" s="36">
+        <v>0</v>
+      </c>
+      <c r="G6" s="36">
+        <v>0</v>
+      </c>
+      <c r="H6" s="36">
+        <v>0</v>
+      </c>
+      <c r="I6" s="36">
+        <v>0</v>
+      </c>
+      <c r="J6" s="36">
+        <v>0</v>
+      </c>
+      <c r="K6" s="36">
+        <v>0</v>
+      </c>
+      <c r="L6" s="36">
+        <v>0</v>
+      </c>
+      <c r="M6" s="36">
+        <v>0</v>
+      </c>
+      <c r="N6" s="36">
+        <v>0</v>
+      </c>
+      <c r="O6" s="36">
+        <v>0</v>
+      </c>
+      <c r="P6" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="36">
         <v>1</v>
       </c>
-      <c r="R6" s="40">
+      <c r="R6" s="36">
         <v>0.20100000000000001</v>
       </c>
       <c r="S6" s="17">
@@ -1922,53 +1990,53 @@
         <f>1.27307*10^5</f>
         <v>127306.99999999999</v>
       </c>
-      <c r="V6" s="41">
+      <c r="V6" s="37">
         <f>1.2810726*10^5</f>
         <v>128107.26</v>
       </c>
-      <c r="W6" s="40">
-        <v>0</v>
-      </c>
-      <c r="X6" s="40">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="40">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="40">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="40">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="40">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="44">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="44">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="44">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="40">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="40">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="40">
+      <c r="W6" s="36">
+        <v>0</v>
+      </c>
+      <c r="X6" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="36">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="36">
         <v>0</v>
       </c>
     </row>
@@ -1988,43 +2056,43 @@
       <c r="E7" s="17">
         <v>0</v>
       </c>
-      <c r="F7" s="40">
-        <v>0</v>
-      </c>
-      <c r="G7" s="40">
-        <v>0</v>
-      </c>
-      <c r="H7" s="40">
-        <v>0</v>
-      </c>
-      <c r="I7" s="40">
-        <v>0</v>
-      </c>
-      <c r="J7" s="40">
-        <v>0</v>
-      </c>
-      <c r="K7" s="40">
-        <v>0</v>
-      </c>
-      <c r="L7" s="40">
-        <v>0</v>
-      </c>
-      <c r="M7" s="40">
-        <v>0</v>
-      </c>
-      <c r="N7" s="40">
-        <v>0</v>
-      </c>
-      <c r="O7" s="40">
-        <v>0</v>
-      </c>
-      <c r="P7" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="40">
-        <v>0</v>
-      </c>
-      <c r="R7" s="40">
+      <c r="F7" s="36">
+        <v>0</v>
+      </c>
+      <c r="G7" s="36">
+        <v>0</v>
+      </c>
+      <c r="H7" s="36">
+        <v>0</v>
+      </c>
+      <c r="I7" s="36">
+        <v>0</v>
+      </c>
+      <c r="J7" s="36">
+        <v>0</v>
+      </c>
+      <c r="K7" s="36">
+        <v>0</v>
+      </c>
+      <c r="L7" s="36">
+        <v>0</v>
+      </c>
+      <c r="M7" s="36">
+        <v>0</v>
+      </c>
+      <c r="N7" s="36">
+        <v>0</v>
+      </c>
+      <c r="O7" s="36">
+        <v>0</v>
+      </c>
+      <c r="P7" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="36">
+        <v>0</v>
+      </c>
+      <c r="R7" s="36">
         <v>0</v>
       </c>
       <c r="S7" s="17">
@@ -2039,49 +2107,49 @@
       <c r="V7" s="17">
         <v>5192.3455999999996</v>
       </c>
-      <c r="W7" s="40">
-        <v>0</v>
-      </c>
-      <c r="X7" s="40">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="40">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="44">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="44">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="44">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="40">
+      <c r="W7" s="36">
+        <v>0</v>
+      </c>
+      <c r="X7" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="36">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="36">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="36">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="36">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="36">
         <v>0</v>
       </c>
     </row>
@@ -5159,12 +5227,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -5178,6 +5240,12 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5186,10 +5254,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X58"/>
+  <dimension ref="A1:X56"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5305,20 +5373,17 @@
       <c r="X3" s="10"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
@@ -5327,21 +5392,20 @@
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+    <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -5350,23 +5414,35 @@
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>
     </row>
-    <row r="6" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="65"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="65"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
@@ -5376,36 +5452,20 @@
       <c r="X6" s="10"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="M7" s="61"/>
-      <c r="N7" s="61"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -5414,49 +5474,23 @@
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
-        <v>4</v>
-      </c>
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="14">
-        <v>3</v>
-      </c>
-      <c r="E8" s="14">
-        <v>4</v>
-      </c>
-      <c r="F8" s="14">
-        <v>663</v>
-      </c>
-      <c r="G8" s="14">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14">
-        <v>0</v>
-      </c>
-      <c r="I8" s="19">
-        <v>663</v>
-      </c>
-      <c r="J8" s="19">
-        <v>0</v>
-      </c>
-      <c r="K8" s="19">
-        <v>1</v>
-      </c>
-      <c r="L8" s="21">
-        <v>663</v>
-      </c>
-      <c r="M8" s="21">
-        <v>1</v>
-      </c>
-      <c r="N8" s="21">
-        <v>0</v>
-      </c>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -5466,18 +5500,36 @@
       <c r="X8" s="10"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="9"/>
+      <c r="A9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -5486,20 +5538,49 @@
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <v>4</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="14">
+        <v>3</v>
+      </c>
+      <c r="E10" s="14">
+        <v>4</v>
+      </c>
+      <c r="F10" s="14">
+        <v>663</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0</v>
+      </c>
+      <c r="I10" s="19">
+        <v>663</v>
+      </c>
+      <c r="J10" s="19">
+        <v>0</v>
+      </c>
+      <c r="K10" s="19">
+        <v>1</v>
+      </c>
+      <c r="L10" s="21">
+        <v>663</v>
+      </c>
+      <c r="M10" s="21">
+        <v>1</v>
+      </c>
+      <c r="N10" s="21">
+        <v>0</v>
+      </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5509,31 +5590,18 @@
       <c r="X10" s="10"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="9"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5542,40 +5610,20 @@
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
-        <v>2</v>
-      </c>
-      <c r="B12" s="14" t="s">
+    <row r="12" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="14">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14">
-        <v>2</v>
-      </c>
-      <c r="F12" s="14">
-        <v>0</v>
-      </c>
-      <c r="G12" s="14">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <v>0</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0</v>
-      </c>
-      <c r="J12" s="14">
-        <v>0</v>
-      </c>
-      <c r="K12" s="14">
-        <v>1</v>
-      </c>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
@@ -5584,24 +5632,74 @@
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
+      <c r="A14" s="14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="14">
+        <v>0</v>
+      </c>
+      <c r="J14" s="14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="14">
+        <v>1</v>
+      </c>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
@@ -5610,310 +5708,337 @@
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="59" t="s">
+    <row r="15" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+    </row>
+    <row r="17" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-    </row>
-    <row r="16" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+    </row>
+    <row r="18" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C18" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="60" t="s">
+      <c r="F18" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="61" t="s">
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-    </row>
-    <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-    </row>
-    <row r="18" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="9"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-    </row>
-    <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="59" t="s">
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+    </row>
+    <row r="19" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+    </row>
+    <row r="20" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="9"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+    </row>
+    <row r="21" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-    </row>
-    <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+    </row>
+    <row r="22" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B22" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C22" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D22" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E22" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="60" t="s">
+      <c r="F22" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="61" t="s">
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
-    </row>
-    <row r="21" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
+    </row>
+    <row r="23" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="19">
         <v>5</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B23" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C23" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D23" s="19">
         <v>4</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E23" s="19">
         <v>1</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F23" s="19">
         <v>660</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G23" s="19">
         <v>-40</v>
       </c>
-      <c r="H21" s="19">
-        <v>0</v>
-      </c>
-      <c r="I21" s="19">
+      <c r="H23" s="19">
+        <v>0</v>
+      </c>
+      <c r="I23" s="19">
         <v>1</v>
       </c>
-      <c r="J21" s="19">
-        <v>0</v>
-      </c>
-      <c r="K21" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:24" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="59"/>
-    </row>
-    <row r="24" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="J23" s="19">
+        <v>0</v>
+      </c>
+      <c r="K23" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+    </row>
+    <row r="26" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B26" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C26" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="63"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="J24" s="63"/>
-      <c r="K24" s="64"/>
-    </row>
-    <row r="25" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-    </row>
-    <row r="26" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="10"/>
-    </row>
-    <row r="28" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+      <c r="D26" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="9"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+      <c r="X28" s="10"/>
+    </row>
+    <row r="29" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="10"/>
+    </row>
+    <row r="30" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B30" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C30" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D30" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-    </row>
-    <row r="29" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="9"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="10"/>
-      <c r="V30" s="10"/>
-      <c r="W30" s="10"/>
-      <c r="X30" s="10"/>
-    </row>
-    <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="59" t="s">
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>1</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
+      <c r="C31" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -5921,123 +6046,125 @@
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="10"/>
-      <c r="T31" s="10"/>
-      <c r="U31" s="10"/>
-      <c r="V31" s="10"/>
-      <c r="W31" s="10"/>
-      <c r="X31" s="10"/>
-    </row>
-    <row r="32" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+    </row>
+    <row r="33" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="9"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C34" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="E34" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+    </row>
+    <row r="35" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
         <v>1</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B35" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="4">
+      <c r="D35" s="14">
         <v>1</v>
       </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-    </row>
-    <row r="35" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="66"/>
-      <c r="C35" s="66"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="66"/>
-      <c r="F35" s="66"/>
-      <c r="G35" s="67"/>
+      <c r="E35" s="14">
+        <v>0</v>
+      </c>
+      <c r="F35" s="14">
+        <v>0</v>
+      </c>
+      <c r="G35" s="14">
+        <v>0</v>
+      </c>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="9"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
+    </row>
+    <row r="36" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>2</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="14">
+        <v>2</v>
+      </c>
+      <c r="E36" s="14">
+        <v>173.2</v>
+      </c>
+      <c r="F36" s="14">
+        <f>-100</f>
+        <v>-100</v>
+      </c>
+      <c r="G36" s="14">
+        <v>0</v>
+      </c>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
     </row>
     <row r="37" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D37" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E37" s="14">
-        <v>0</v>
+        <v>663</v>
       </c>
       <c r="F37" s="14">
         <v>0</v>
@@ -6045,131 +6172,80 @@
       <c r="G37" s="14">
         <v>0</v>
       </c>
-      <c r="H37" s="12"/>
+      <c r="H37"/>
       <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D38" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E38" s="14">
-        <v>173.2</v>
+        <v>763</v>
       </c>
       <c r="F38" s="14">
-        <f>-100</f>
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="G38" s="14">
         <v>0</v>
       </c>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14">
-        <v>3</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D39" s="14">
-        <v>3</v>
-      </c>
-      <c r="E39" s="14">
-        <v>663</v>
-      </c>
-      <c r="F39" s="14">
-        <v>0</v>
-      </c>
-      <c r="G39" s="14">
-        <v>0</v>
-      </c>
-      <c r="H39"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
-        <v>4</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="14">
-        <v>4</v>
-      </c>
-      <c r="E40" s="14">
-        <v>763</v>
-      </c>
-      <c r="F40" s="14">
-        <v>0</v>
-      </c>
-      <c r="G40" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M42" t="s">
+      <c r="M40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-    </row>
-    <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="56" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A8:N8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A33:G33"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Spherical,Universal,Revolute,Translation,Cylindrical,Simple,Ground,Driver"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B46:B1032 B37:B40" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:B1030 B35:B38" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Spherical,Universal,Revolute,Cylindrical,Translation,Simple,Driver,Ground,Point"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6198,18 +6274,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -6227,11 +6303,11 @@
       <c r="E2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="69"/>
       <c r="I2" s="26" t="s">
         <v>56</v>
       </c>
@@ -6256,7 +6332,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -6276,10 +6352,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1356001A-570B-4774-AE32-331534C6A696}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6288,179 +6364,363 @@
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="9" max="9" width="36" customWidth="1"/>
-    <col min="16" max="16" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+    </row>
+    <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="80" t="s">
+        <v>126</v>
+      </c>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E3" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="60" t="s">
+      <c r="F3" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="28" t="s">
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="J3" s="72" t="s">
+        <v>127</v>
+      </c>
+      <c r="K3" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="L3" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="M3" s="79" t="s">
+        <v>130</v>
+      </c>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79" t="s">
+        <v>131</v>
+      </c>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="79" t="s">
+        <v>132</v>
+      </c>
+      <c r="R3" s="79"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="27"/>
+    </row>
+    <row r="7" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="70" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="71"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="71"/>
+      <c r="Q7" s="71"/>
+      <c r="R7" s="71"/>
+    </row>
+    <row r="8" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="81" t="s">
+        <v>125</v>
+      </c>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="72" t="s">
+        <v>127</v>
+      </c>
+      <c r="K9" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="L9" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="M9" s="73" t="s">
+        <v>130</v>
+      </c>
+      <c r="N9" s="73"/>
+      <c r="O9" s="73" t="s">
+        <v>131</v>
+      </c>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="R9" s="73"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="13" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="63"/>
+    </row>
+    <row r="14" spans="1:18" s="78" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="74" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="75" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-    </row>
-    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="65" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="67"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="J12" s="45" t="s">
+      <c r="J14" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45" t="s">
+      <c r="K14" s="77"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="77" t="s">
+        <v>84</v>
+      </c>
+      <c r="N14" s="77"/>
+      <c r="O14" s="77"/>
+      <c r="P14" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="37" t="s">
-        <v>88</v>
-      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="A11:P11"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:I6"/>
+  <mergeCells count="18">
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="J2:R2"/>
+    <mergeCell ref="A7:R7"/>
+    <mergeCell ref="J8:R8"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="A13:P13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Spring and Dampers Non Linear
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74E3AF9-C10A-4FD4-9DD0-5F431B86EFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D1166F-B8D7-41C4-8BA8-D328D46EE9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="134">
   <si>
     <t>Mass</t>
   </si>
@@ -412,10 +412,38 @@
     <t>Linear - Damping Coefficient</t>
   </si>
   <si>
-    <t>@(x) Non Linear Force Function (x-Vel)</t>
-  </si>
-  <si>
     <t>@(x) Non Linear Force Function (x-Displ)</t>
+  </si>
+  <si>
+    <t>Function 1</t>
+  </si>
+  <si>
+    <t>Function 2</t>
+  </si>
+  <si>
+    <t>Function 3</t>
+  </si>
+  <si>
+    <t>@(dx) Non Linear Force Function (dx-Vel)</t>
+  </si>
+  <si>
+    <t>Numb of Functions</t>
+  </si>
+  <si>
+    <t>Function  Interval</t>
+  </si>
+  <si>
+    <t>Function Interval</t>
+  </si>
+  <si>
+    <t>The Non Linear Force Function can be divided into three functions with different intervals. 
+When Defining the Interval the Matlab will assume the values as:
+Function 1 from - inf to first interval value ( and = )
+Function 2 between the two defined values
+Function 3 from the second value (and = ) to +inf
+It is possible to define only 1 or 2 functions.
+With 1 Function matlab will ignore the interval
+with 2 Functions matlab will use only the first value and use it to define the Boundary between the 2 functions.</t>
   </si>
 </sst>
 </file>
@@ -509,7 +537,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -600,6 +628,19 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -620,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,9 +741,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -730,7 +777,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -742,6 +792,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -763,6 +816,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -775,13 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,7 +846,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -802,15 +864,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -826,35 +879,47 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1255,176 +1320,176 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="49"/>
-      <c r="I2" s="45" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+      <c r="I2" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="45"/>
-      <c r="L2" s="45" t="s">
+      <c r="J2" s="49"/>
+      <c r="L2" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="45"/>
+      <c r="M2" s="49"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="55"/>
       <c r="D3" s="30">
         <v>2</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="L3" s="36" t="s">
+      <c r="L3" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="38" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="46"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="30">
         <v>0.5</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="36" t="s">
+      <c r="I4" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="L4" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" s="36" t="s">
+      <c r="L4" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="38" t="s">
         <v>110</v>
       </c>
       <c r="S4" s="13"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="46"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="30" t="s">
         <v>91</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="L5" s="36" t="s">
+      <c r="L5" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="M5" s="36" t="s">
+      <c r="M5" s="38" t="s">
         <v>111</v>
       </c>
       <c r="S5" s="13"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="46"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="30"/>
       <c r="E6" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="36" t="s">
+      <c r="L6" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="M6" s="38" t="s">
         <v>22</v>
       </c>
       <c r="S6" s="13"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="30"/>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I7" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="J7" s="36" t="s">
+      <c r="J7" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="L7" s="36" t="s">
+      <c r="L7" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="M7" s="36" t="s">
+      <c r="M7" s="38" t="s">
         <v>114</v>
       </c>
       <c r="S7" s="13"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="J8" s="36" t="s">
+      <c r="J8" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="L8" s="36" t="s">
+      <c r="L8" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="M8" s="36" t="s">
+      <c r="M8" s="38" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="M9" s="39" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1449,7 +1514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AI18" sqref="AI18"/>
     </sheetView>
   </sheetViews>
@@ -1469,118 +1534,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="59"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45" t="s">
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45" t="s">
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45" t="s">
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="45"/>
-      <c r="AJ1" s="45"/>
-      <c r="AK1" s="45"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="49"/>
+      <c r="AG1" s="49"/>
+      <c r="AH1" s="49"/>
+      <c r="AI1" s="49"/>
+      <c r="AJ1" s="49"/>
+      <c r="AK1" s="49"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="54" t="s">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54" t="s">
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="45" t="s">
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45" t="s">
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="55" t="s">
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="54" t="s">
+      <c r="S2" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="45" t="s">
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
       <c r="Z2" s="56" t="s">
         <v>102</v>
       </c>
       <c r="AA2" s="57"/>
       <c r="AB2" s="58"/>
-      <c r="AC2" s="45" t="s">
+      <c r="AC2" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="45"/>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="45" t="s">
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45" t="s">
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
+      <c r="AI2" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="AJ2" s="45"/>
-      <c r="AK2" s="45"/>
+      <c r="AJ2" s="49"/>
+      <c r="AK2" s="49"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
@@ -1634,8 +1699,8 @@
       <c r="Q3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="55"/>
-      <c r="S3" s="53"/>
+      <c r="R3" s="62"/>
+      <c r="S3" s="60"/>
       <c r="T3" s="17" t="s">
         <v>69</v>
       </c>
@@ -1681,13 +1746,13 @@
       <c r="AH3" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="AI3" s="32" t="s">
+      <c r="AI3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="AJ3" s="32" t="s">
+      <c r="AJ3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="AK3" s="32" t="s">
+      <c r="AK3" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1707,43 +1772,43 @@
       <c r="E4" s="17">
         <v>0</v>
       </c>
-      <c r="F4" s="34">
-        <v>0</v>
-      </c>
-      <c r="G4" s="34">
-        <v>0</v>
-      </c>
-      <c r="H4" s="34">
-        <v>0</v>
-      </c>
-      <c r="I4" s="34">
-        <v>0</v>
-      </c>
-      <c r="J4" s="34">
-        <v>0</v>
-      </c>
-      <c r="K4" s="34">
-        <v>0</v>
-      </c>
-      <c r="L4" s="34">
-        <v>0</v>
-      </c>
-      <c r="M4" s="34">
-        <v>0</v>
-      </c>
-      <c r="N4" s="34">
-        <v>0</v>
-      </c>
-      <c r="O4" s="34">
-        <v>0</v>
-      </c>
-      <c r="P4" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="34">
-        <v>0</v>
-      </c>
-      <c r="R4" s="34">
+      <c r="F4" s="36">
+        <v>0</v>
+      </c>
+      <c r="G4" s="36">
+        <v>0</v>
+      </c>
+      <c r="H4" s="36">
+        <v>0</v>
+      </c>
+      <c r="I4" s="36">
+        <v>0</v>
+      </c>
+      <c r="J4" s="36">
+        <v>0</v>
+      </c>
+      <c r="K4" s="36">
+        <v>0</v>
+      </c>
+      <c r="L4" s="36">
+        <v>0</v>
+      </c>
+      <c r="M4" s="36">
+        <v>0</v>
+      </c>
+      <c r="N4" s="36">
+        <v>0</v>
+      </c>
+      <c r="O4" s="36">
+        <v>0</v>
+      </c>
+      <c r="P4" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="36">
+        <v>0</v>
+      </c>
+      <c r="R4" s="36">
         <v>0</v>
       </c>
       <c r="S4" s="17">
@@ -1758,49 +1823,49 @@
       <c r="V4" s="17">
         <v>0</v>
       </c>
-      <c r="W4" s="34">
-        <v>0</v>
-      </c>
-      <c r="X4" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="38">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="38">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="38">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="38">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="38">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="38">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="34">
+      <c r="W4" s="36">
+        <v>0</v>
+      </c>
+      <c r="X4" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="36">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="36">
         <v>0</v>
       </c>
     </row>
@@ -1820,43 +1885,43 @@
       <c r="E5" s="24">
         <v>0</v>
       </c>
-      <c r="F5" s="34">
-        <v>0</v>
-      </c>
-      <c r="G5" s="34">
-        <v>0</v>
-      </c>
-      <c r="H5" s="34">
-        <v>0</v>
-      </c>
-      <c r="I5" s="34">
-        <v>0</v>
-      </c>
-      <c r="J5" s="34">
-        <v>0</v>
-      </c>
-      <c r="K5" s="34">
-        <v>0</v>
-      </c>
-      <c r="L5" s="34">
-        <v>0</v>
-      </c>
-      <c r="M5" s="34">
-        <v>0</v>
-      </c>
-      <c r="N5" s="34">
-        <v>0</v>
-      </c>
-      <c r="O5" s="34">
-        <v>0</v>
-      </c>
-      <c r="P5" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="34">
+      <c r="F5" s="36">
+        <v>0</v>
+      </c>
+      <c r="G5" s="36">
+        <v>0</v>
+      </c>
+      <c r="H5" s="36">
+        <v>0</v>
+      </c>
+      <c r="I5" s="36">
+        <v>0</v>
+      </c>
+      <c r="J5" s="36">
+        <v>0</v>
+      </c>
+      <c r="K5" s="36">
+        <v>0</v>
+      </c>
+      <c r="L5" s="36">
+        <v>0</v>
+      </c>
+      <c r="M5" s="36">
+        <v>0</v>
+      </c>
+      <c r="N5" s="36">
+        <v>0</v>
+      </c>
+      <c r="O5" s="36">
+        <v>0</v>
+      </c>
+      <c r="P5" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="36">
         <v>1</v>
       </c>
-      <c r="R5" s="34">
+      <c r="R5" s="36">
         <v>-0.52359999999999995</v>
       </c>
       <c r="S5" s="17">
@@ -1871,49 +1936,49 @@
       <c r="V5" s="17">
         <v>1312.9336000000001</v>
       </c>
-      <c r="W5" s="34">
-        <v>0</v>
-      </c>
-      <c r="X5" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="34">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="38">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="38">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="38">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="38">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="38">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="38">
+      <c r="W5" s="36">
+        <v>0</v>
+      </c>
+      <c r="X5" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="36">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="36">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="36">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="40">
         <v>5</v>
       </c>
-      <c r="AI5" s="34">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="34">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="34">
+      <c r="AI5" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="36">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="36">
         <v>0</v>
       </c>
     </row>
@@ -1933,43 +1998,43 @@
       <c r="E6" s="24">
         <v>0</v>
       </c>
-      <c r="F6" s="34">
-        <v>0</v>
-      </c>
-      <c r="G6" s="34">
-        <v>0</v>
-      </c>
-      <c r="H6" s="34">
-        <v>0</v>
-      </c>
-      <c r="I6" s="34">
-        <v>0</v>
-      </c>
-      <c r="J6" s="34">
-        <v>0</v>
-      </c>
-      <c r="K6" s="34">
-        <v>0</v>
-      </c>
-      <c r="L6" s="34">
-        <v>0</v>
-      </c>
-      <c r="M6" s="34">
-        <v>0</v>
-      </c>
-      <c r="N6" s="34">
-        <v>0</v>
-      </c>
-      <c r="O6" s="34">
-        <v>0</v>
-      </c>
-      <c r="P6" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="34">
+      <c r="F6" s="36">
+        <v>0</v>
+      </c>
+      <c r="G6" s="36">
+        <v>0</v>
+      </c>
+      <c r="H6" s="36">
+        <v>0</v>
+      </c>
+      <c r="I6" s="36">
+        <v>0</v>
+      </c>
+      <c r="J6" s="36">
+        <v>0</v>
+      </c>
+      <c r="K6" s="36">
+        <v>0</v>
+      </c>
+      <c r="L6" s="36">
+        <v>0</v>
+      </c>
+      <c r="M6" s="36">
+        <v>0</v>
+      </c>
+      <c r="N6" s="36">
+        <v>0</v>
+      </c>
+      <c r="O6" s="36">
+        <v>0</v>
+      </c>
+      <c r="P6" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="36">
         <v>1</v>
       </c>
-      <c r="R6" s="34">
+      <c r="R6" s="36">
         <v>0.20100000000000001</v>
       </c>
       <c r="S6" s="17">
@@ -1982,53 +2047,53 @@
         <f>1.27307*10^5</f>
         <v>127306.99999999999</v>
       </c>
-      <c r="V6" s="35">
+      <c r="V6" s="37">
         <f>1.2810726*10^5</f>
         <v>128107.26</v>
       </c>
-      <c r="W6" s="34">
-        <v>0</v>
-      </c>
-      <c r="X6" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="38">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="38">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="38">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="38">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="38">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="38">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="34">
+      <c r="W6" s="36">
+        <v>0</v>
+      </c>
+      <c r="X6" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="36">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="36">
         <v>0</v>
       </c>
     </row>
@@ -2048,43 +2113,43 @@
       <c r="E7" s="17">
         <v>0</v>
       </c>
-      <c r="F7" s="34">
-        <v>0</v>
-      </c>
-      <c r="G7" s="34">
-        <v>0</v>
-      </c>
-      <c r="H7" s="34">
-        <v>0</v>
-      </c>
-      <c r="I7" s="34">
-        <v>0</v>
-      </c>
-      <c r="J7" s="34">
-        <v>0</v>
-      </c>
-      <c r="K7" s="34">
-        <v>0</v>
-      </c>
-      <c r="L7" s="34">
-        <v>0</v>
-      </c>
-      <c r="M7" s="34">
-        <v>0</v>
-      </c>
-      <c r="N7" s="34">
-        <v>0</v>
-      </c>
-      <c r="O7" s="34">
-        <v>0</v>
-      </c>
-      <c r="P7" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="34">
-        <v>0</v>
-      </c>
-      <c r="R7" s="34">
+      <c r="F7" s="36">
+        <v>0</v>
+      </c>
+      <c r="G7" s="36">
+        <v>0</v>
+      </c>
+      <c r="H7" s="36">
+        <v>0</v>
+      </c>
+      <c r="I7" s="36">
+        <v>0</v>
+      </c>
+      <c r="J7" s="36">
+        <v>0</v>
+      </c>
+      <c r="K7" s="36">
+        <v>0</v>
+      </c>
+      <c r="L7" s="36">
+        <v>0</v>
+      </c>
+      <c r="M7" s="36">
+        <v>0</v>
+      </c>
+      <c r="N7" s="36">
+        <v>0</v>
+      </c>
+      <c r="O7" s="36">
+        <v>0</v>
+      </c>
+      <c r="P7" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="36">
+        <v>0</v>
+      </c>
+      <c r="R7" s="36">
         <v>0</v>
       </c>
       <c r="S7" s="17">
@@ -2099,49 +2164,49 @@
       <c r="V7" s="17">
         <v>5192.3455999999996</v>
       </c>
-      <c r="W7" s="34">
-        <v>0</v>
-      </c>
-      <c r="X7" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="34">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="38">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="38">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="38">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="38">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="38">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="38">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="34">
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="34">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="34">
+      <c r="W7" s="36">
+        <v>0</v>
+      </c>
+      <c r="X7" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="36">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="36">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="36">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="36">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="36">
         <v>0</v>
       </c>
     </row>
@@ -5219,12 +5284,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -5238,6 +5297,12 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5269,16 +5334,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -5309,11 +5374,11 @@
       <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -5385,19 +5450,19 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -5422,16 +5487,16 @@
       <c r="E6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="62" t="s">
+      <c r="F6" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="63"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="62" t="s">
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="J6" s="63"/>
-      <c r="K6" s="64"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="71"/>
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
@@ -5467,22 +5532,22 @@
       <c r="X7" s="10"/>
     </row>
     <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
-      <c r="M8" s="59"/>
-      <c r="N8" s="59"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -5507,21 +5572,21 @@
       <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="61" t="s">
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61" t="s">
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="61"/>
-      <c r="N9" s="61"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -5603,19 +5668,19 @@
       <c r="X11" s="10"/>
     </row>
     <row r="12" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
@@ -5640,16 +5705,16 @@
       <c r="E13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="60" t="s">
+      <c r="F13" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="61" t="s">
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -5727,19 +5792,19 @@
       <c r="X16" s="10"/>
     </row>
     <row r="17" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
@@ -5764,16 +5829,16 @@
       <c r="E18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="61" t="s">
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
     </row>
     <row r="19" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
@@ -5810,19 +5875,19 @@
       <c r="X20" s="10"/>
     </row>
     <row r="21" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
@@ -5847,16 +5912,16 @@
       <c r="E22" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="61" t="s">
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
     </row>
     <row r="23" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
@@ -5895,14 +5960,14 @@
     </row>
     <row r="24" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="59" t="s">
+      <c r="A25" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
@@ -5976,12 +6041,12 @@
       <c r="X28" s="10"/>
     </row>
     <row r="29" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -6053,15 +6118,15 @@
       <c r="K32" s="11"/>
     </row>
     <row r="33" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="65" t="s">
+      <c r="A33" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="67"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="68"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
       <c r="J33" s="10"/>
@@ -6081,11 +6146,11 @@
       <c r="D34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="61" t="s">
+      <c r="E34" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="F34" s="61"/>
-      <c r="G34" s="61"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
       <c r="J34" s="10"/>
@@ -6209,19 +6274,6 @@
     <row r="56" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="A8:N8"/>
@@ -6231,6 +6283,19 @@
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A33:G33"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -6266,18 +6331,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -6295,11 +6360,11 @@
       <c r="E2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74"/>
       <c r="I2" s="26" t="s">
         <v>56</v>
       </c>
@@ -6344,10 +6409,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1356001A-570B-4774-AE32-331534C6A696}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6359,7 +6424,7 @@
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="19.140625" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" customWidth="1"/>
     <col min="15" max="15" width="12.28515625" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" customWidth="1"/>
@@ -6367,62 +6432,101 @@
     <col min="18" max="18" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+    <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-    </row>
-    <row r="2" spans="1:16" s="80" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+    </row>
+    <row r="2" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="84" t="s">
+        <v>125</v>
+      </c>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="86"/>
+      <c r="R2" s="90" t="s">
+        <v>133</v>
+      </c>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="90"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="77" t="s">
+      <c r="E3" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F3" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79" t="s">
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="J2" s="75" t="s">
+      <c r="J3" s="44" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="K3" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="L3" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="M3" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="N3" s="79" t="s">
+        <v>132</v>
+      </c>
+      <c r="O3" s="79"/>
+      <c r="R3" s="90"/>
+      <c r="S3" s="90"/>
+      <c r="T3" s="90"/>
+      <c r="U3" s="90"/>
+      <c r="V3" s="90"/>
+      <c r="W3" s="90"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -6430,179 +6534,301 @@
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="27"/>
-    </row>
-    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="81" t="s">
+      <c r="I4" s="32"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="90"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="90"/>
+      <c r="T5" s="90"/>
+      <c r="U5" s="90"/>
+      <c r="V5" s="90"/>
+      <c r="W5" s="90"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R6" s="90"/>
+      <c r="S6" s="90"/>
+      <c r="T6" s="90"/>
+      <c r="U6" s="90"/>
+      <c r="V6" s="90"/>
+      <c r="W6" s="90"/>
+    </row>
+    <row r="7" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-    </row>
-    <row r="7" spans="1:16" s="44" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="R7" s="90"/>
+      <c r="S7" s="90"/>
+      <c r="T7" s="90"/>
+      <c r="U7" s="90"/>
+      <c r="V7" s="90"/>
+      <c r="W7" s="90"/>
+    </row>
+    <row r="8" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="87" t="s">
+        <v>129</v>
+      </c>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="89"/>
+      <c r="R8" s="90"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="90"/>
+      <c r="U8" s="90"/>
+      <c r="V8" s="90"/>
+      <c r="W8" s="90"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B9" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C9" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="74" t="s">
+      <c r="F9" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="43" t="s">
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="J7" s="76" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="27"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="41"/>
-    </row>
-    <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="65" t="s">
+      <c r="J9" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="K9" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="L9" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="M9" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="N9" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="O9" s="78"/>
+      <c r="R9" s="90"/>
+      <c r="S9" s="90"/>
+      <c r="T9" s="90"/>
+      <c r="U9" s="90"/>
+      <c r="V9" s="90"/>
+      <c r="W9" s="90"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="27"/>
+      <c r="R10" s="90"/>
+      <c r="S10" s="90"/>
+      <c r="T10" s="90"/>
+      <c r="U10" s="90"/>
+      <c r="V10" s="90"/>
+      <c r="W10" s="90"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="R11" s="90"/>
+      <c r="S11" s="90"/>
+      <c r="T11" s="90"/>
+      <c r="U11" s="90"/>
+      <c r="V11" s="90"/>
+      <c r="W11" s="90"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R12" s="90"/>
+      <c r="S12" s="90"/>
+      <c r="T12" s="90"/>
+      <c r="U12" s="90"/>
+      <c r="V12" s="90"/>
+      <c r="W12" s="90"/>
+    </row>
+    <row r="13" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="67"/>
-    </row>
-    <row r="12" spans="1:16" s="44" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="68"/>
+      <c r="R13" s="90"/>
+      <c r="S13" s="90"/>
+      <c r="T13" s="90"/>
+      <c r="U13" s="90"/>
+      <c r="V13" s="90"/>
+      <c r="W13" s="90"/>
+    </row>
+    <row r="14" spans="1:23" s="47" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B14" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C14" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D14" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E14" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="74" t="s">
+      <c r="F14" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="43" t="s">
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="73" t="s">
+      <c r="J14" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="73" t="s">
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="N12" s="73"/>
-      <c r="O12" s="73"/>
-      <c r="P12" s="40" t="s">
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="42" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="A11:P11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A6:J6"/>
+  <mergeCells count="15">
+    <mergeCell ref="R2:W13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="A13:P13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="A7:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes to Plots and Some Bug Fixes
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/template_mbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ABEE2D-41EC-4AD9-9BBD-06867593704E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5B7C8A-791A-4853-841A-BBA1647FE666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="175">
   <si>
     <t>Mass</t>
   </si>
@@ -585,6 +585,12 @@
   </si>
   <si>
     <t xml:space="preserve"> @(t) Function</t>
+  </si>
+  <si>
+    <t>Force Element</t>
+  </si>
+  <si>
+    <t>Suspension Point</t>
   </si>
 </sst>
 </file>
@@ -854,7 +860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -882,7 +888,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1157,49 +1162,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1285,6 +1287,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>924832</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1A21537-C858-258D-47C1-8AACE29B3FF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7505701" y="4200525"/>
+          <a:ext cx="3658506" cy="3019425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1584,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
-  <dimension ref="B2:S27"/>
+  <dimension ref="B2:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,543 +1647,626 @@
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="15" max="15" width="19.85546875" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="3.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="111" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="70"/>
+      <c r="J2" s="122" t="s">
+        <v>168</v>
+      </c>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="122"/>
+      <c r="Q2" s="122"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="109">
+      <c r="C3" s="110"/>
+      <c r="D3" s="107">
         <v>2</v>
       </c>
-      <c r="E3" s="109" t="s">
+      <c r="E3" s="107" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="111" t="s">
+      <c r="J3" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="K3" s="106"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="105" t="s">
+        <v>142</v>
+      </c>
+      <c r="N3" s="106"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q3" s="48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="109">
+      <c r="C4" s="110"/>
+      <c r="D4" s="107">
         <v>0.05</v>
       </c>
-      <c r="E4" s="109" t="s">
+      <c r="E4" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="S4" s="13"/>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="111" t="s">
+      <c r="J4" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="K4" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="L4" s="112"/>
+      <c r="M4" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="N4" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="O4" s="72"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="115"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="109" t="s">
+      <c r="C5" s="110"/>
+      <c r="D5" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="109" t="s">
+      <c r="E5" s="107" t="s">
         <v>78</v>
       </c>
-      <c r="L5" s="69" t="s">
-        <v>168</v>
-      </c>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="71"/>
-      <c r="S5" s="13"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="111" t="s">
+      <c r="J5" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="L5" s="112"/>
+      <c r="M5" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="72"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="115"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="109" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109" t="s">
+      <c r="C6" s="110"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="L6" s="106" t="s">
-        <v>115</v>
-      </c>
-      <c r="M6" s="106"/>
-      <c r="N6" s="113"/>
-      <c r="O6" s="107" t="s">
-        <v>142</v>
-      </c>
-      <c r="P6" s="108"/>
-      <c r="S6" s="13"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="111" t="s">
+      <c r="J6" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="K6" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="L6" s="112"/>
+      <c r="M6" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="N6" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="O6" s="72"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="115"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="109" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="112"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="110" t="s">
+      <c r="C7" s="110"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="108" t="s">
         <v>118</v>
       </c>
-      <c r="L7" s="49" t="s">
+      <c r="J7" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="K7" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="112"/>
+      <c r="M7" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="72"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="115"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="109" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="110"/>
+      <c r="D8" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="108" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="K8" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="L8" s="112"/>
+      <c r="M8" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="72"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="109" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="110"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="108" t="s">
+        <v>135</v>
+      </c>
+      <c r="J9" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="K9" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="L9" s="112"/>
+      <c r="M9" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="72"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J10" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="L10" s="112"/>
+      <c r="M10" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="72"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J11" s="116"/>
+      <c r="K11" s="117"/>
+      <c r="L11" s="112"/>
+      <c r="M11" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="N11" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="O11" s="72"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="119"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="N12" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="O12" s="72"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="54" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" s="54"/>
+      <c r="D13" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="J13" s="118"/>
+      <c r="K13" s="119"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="72"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" s="54"/>
+      <c r="D14" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="121"/>
+      <c r="L14" s="112"/>
+      <c r="M14" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="N14" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="O14" s="72"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="54" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="54"/>
+      <c r="D15" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="J15" s="105" t="s">
+        <v>104</v>
+      </c>
+      <c r="K15" s="106"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="O15" s="72"/>
+      <c r="P15" s="48"/>
+      <c r="Q15" s="48"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="54"/>
+      <c r="D16" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="72"/>
+      <c r="J16" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="M7" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="N7" s="114"/>
-      <c r="O7" s="47" t="s">
-        <v>143</v>
-      </c>
-      <c r="P7" s="49" t="s">
+      <c r="K16" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="L16" s="112"/>
+      <c r="M16" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="N16" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="O16" s="72"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="48"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="C17" s="54"/>
+      <c r="D17" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="72"/>
+      <c r="J17" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="L17" s="112"/>
+      <c r="M17" s="105" t="s">
+        <v>163</v>
+      </c>
+      <c r="N17" s="106"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="66" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="67"/>
+      <c r="D18" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="J18" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="L18" s="112"/>
+      <c r="M18" s="114" t="s">
+        <v>173</v>
+      </c>
+      <c r="N18" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="S7" s="13"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="111" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="112"/>
-      <c r="D8" s="109" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="110" t="s">
-        <v>97</v>
-      </c>
-      <c r="L8" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="M8" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="N8" s="114"/>
-      <c r="O8" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" s="49" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="111" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" s="112"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="110" t="s">
+      <c r="O18" s="72"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="67"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="L9" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="M9" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="N9" s="114"/>
-      <c r="O9" s="49" t="s">
-        <v>145</v>
-      </c>
-      <c r="P9" s="49" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="L10" s="49" t="s">
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="J19" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="M10" s="49" t="s">
+      <c r="K19" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="114"/>
-      <c r="O10" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="P10" s="49" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="L11" s="49" t="s">
+      <c r="L19" s="112"/>
+      <c r="M19" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="N19" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="O19" s="72"/>
+      <c r="P19" s="48"/>
+      <c r="Q19" s="48"/>
+    </row>
+    <row r="20" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="58"/>
+      <c r="D20" s="45">
+        <v>2</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="G20" s="53"/>
+      <c r="H20" s="52"/>
+      <c r="J20" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="M11" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="N11" s="114"/>
-      <c r="O11" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="P11" s="49" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="56" t="s">
-        <v>151</v>
-      </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="L12" s="49" t="s">
+      <c r="K20" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="L20" s="112"/>
+      <c r="M20" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="N20" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="O20" s="72"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="59"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="45">
+        <v>3</v>
+      </c>
+      <c r="E21" s="64"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="52"/>
+      <c r="J21" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="M12" s="49" t="s">
+      <c r="K21" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="N12" s="114"/>
-      <c r="O12" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="P12" s="49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="L13" s="33" t="s">
+      <c r="L21" s="112"/>
+      <c r="M21" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="N21" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="O21" s="72"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="59"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="45">
+        <v>4</v>
+      </c>
+      <c r="E22" s="64"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="52"/>
+      <c r="J22" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="M13" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="N13" s="114"/>
-      <c r="O13" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="P13" s="49" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="55" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="L14" s="116"/>
-      <c r="M14" s="113"/>
-      <c r="N14" s="114"/>
-      <c r="O14" s="49" t="s">
-        <v>147</v>
-      </c>
-      <c r="P14" s="49" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="55" t="s">
-        <v>157</v>
-      </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="E15" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="L15" s="117"/>
-      <c r="M15" s="114"/>
-      <c r="N15" s="114"/>
-      <c r="O15" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="P15" s="49" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="55" t="s">
-        <v>159</v>
-      </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="L16" s="117"/>
-      <c r="M16" s="114"/>
-      <c r="N16" s="114"/>
-      <c r="O16" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="P16" s="49" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="55" t="s">
-        <v>158</v>
-      </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="L17" s="118"/>
-      <c r="M17" s="115"/>
-      <c r="N17" s="114"/>
-      <c r="O17" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="P17" s="49" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="67" t="s">
-        <v>155</v>
-      </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="L18" s="106" t="s">
-        <v>104</v>
-      </c>
-      <c r="M18" s="106"/>
-      <c r="N18" s="114"/>
-      <c r="O18" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="P18" s="49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="L19" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="M19" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="N19" s="114"/>
-      <c r="O19" s="49" t="s">
-        <v>150</v>
-      </c>
-      <c r="P19" s="49" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="58" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="46">
-        <v>2</v>
-      </c>
-      <c r="E20" s="64" t="s">
-        <v>160</v>
-      </c>
-      <c r="F20" s="54" t="s">
-        <v>161</v>
-      </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53"/>
-      <c r="L20" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="M20" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="N20" s="114"/>
-      <c r="O20" s="119"/>
-      <c r="P20" s="120"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="60"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53"/>
-      <c r="L21" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="M21" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="N21" s="114"/>
-      <c r="O21" s="106" t="s">
-        <v>163</v>
-      </c>
-      <c r="P21" s="106"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="60"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="53"/>
-      <c r="L22" s="49" t="s">
-        <v>107</v>
-      </c>
+      <c r="K22" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="L22" s="113"/>
       <c r="M22" s="49" t="s">
-        <v>22</v>
-      </c>
-      <c r="N22" s="114"/>
-      <c r="O22" s="50" t="s">
-        <v>164</v>
-      </c>
-      <c r="P22" s="50" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="60"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="53"/>
-      <c r="L23" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="M23" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="N23" s="114"/>
-      <c r="O23" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="P23" s="50" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="60"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="53"/>
-      <c r="L24" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="M24" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="N24" s="114"/>
-      <c r="O24" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="P24" s="50" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="60"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="53"/>
-      <c r="L25" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="M25" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="N25" s="115"/>
-      <c r="O25" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="P25" s="49" t="s">
+      <c r="N22" s="48" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="60"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="53"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="62"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="53"/>
+      <c r="O22" s="72"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="59"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="52"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="59"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="52"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="59"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="52"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="59"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="52"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="61"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="L14:M17"/>
-    <mergeCell ref="N6:N25"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="L5:P5"/>
-    <mergeCell ref="O6:P6"/>
+  <mergeCells count="27">
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:L22"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:O22"/>
+    <mergeCell ref="J2:Q2"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L6:M6"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B2:E2"/>
@@ -2152,6 +2286,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2179,679 +2314,679 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="73"/>
-      <c r="B1" s="73"/>
-      <c r="C1" s="55" t="s">
+      <c r="A1" s="72"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55" t="s">
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55" t="s">
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55" t="s">
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55" t="s">
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
-      <c r="AI1" s="55"/>
-      <c r="AJ1" s="55"/>
-      <c r="AK1" s="55"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="75" t="s">
+      <c r="A2" s="72"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75" t="s">
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75" t="s">
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="55" t="s">
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55" t="s">
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="54" t="s">
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="75" t="s">
+      <c r="S2" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="55" t="s">
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="67" t="s">
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="AA2" s="72"/>
-      <c r="AB2" s="68"/>
-      <c r="AC2" s="55" t="s">
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="67"/>
+      <c r="AC2" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="55" t="s">
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
+      <c r="AF2" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="AG2" s="55"/>
-      <c r="AH2" s="55"/>
-      <c r="AI2" s="55" t="s">
+      <c r="AG2" s="54"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="AJ2" s="55"/>
-      <c r="AK2" s="55"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="54"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="17" t="s">
+      <c r="R3" s="53"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="U3" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="V3" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="W3" s="29" t="s">
+      <c r="W3" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="X3" s="29" t="s">
+      <c r="X3" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="Y3" s="29" t="s">
+      <c r="Y3" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="Z3" s="29" t="s">
+      <c r="Z3" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="AA3" s="29" t="s">
+      <c r="AA3" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="AB3" s="29" t="s">
+      <c r="AB3" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="AC3" s="29" t="s">
+      <c r="AC3" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="AD3" s="29" t="s">
+      <c r="AD3" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="AE3" s="29" t="s">
+      <c r="AE3" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="AF3" s="29" t="s">
+      <c r="AF3" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="AG3" s="29" t="s">
+      <c r="AG3" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="AH3" s="29" t="s">
+      <c r="AH3" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="AI3" s="30" t="s">
+      <c r="AI3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="AJ3" s="30" t="s">
+      <c r="AJ3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="AK3" s="30" t="s">
+      <c r="AK3" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="16">
         <v>1</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="17">
-        <v>0</v>
-      </c>
-      <c r="D4" s="17">
-        <v>0</v>
-      </c>
-      <c r="E4" s="17">
-        <v>0</v>
-      </c>
-      <c r="F4" s="31">
-        <v>0</v>
-      </c>
-      <c r="G4" s="31">
-        <v>0</v>
-      </c>
-      <c r="H4" s="31">
-        <v>0</v>
-      </c>
-      <c r="I4" s="31">
-        <v>0</v>
-      </c>
-      <c r="J4" s="31">
-        <v>0</v>
-      </c>
-      <c r="K4" s="31">
-        <v>0</v>
-      </c>
-      <c r="L4" s="31">
-        <v>0</v>
-      </c>
-      <c r="M4" s="31">
-        <v>0</v>
-      </c>
-      <c r="N4" s="31">
-        <v>0</v>
-      </c>
-      <c r="O4" s="31">
-        <v>0</v>
-      </c>
-      <c r="P4" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="31">
-        <v>0</v>
-      </c>
-      <c r="R4" s="31">
-        <v>0</v>
-      </c>
-      <c r="S4" s="17">
-        <v>0</v>
-      </c>
-      <c r="T4" s="17">
-        <v>0</v>
-      </c>
-      <c r="U4" s="17">
-        <v>0</v>
-      </c>
-      <c r="V4" s="17">
-        <v>0</v>
-      </c>
-      <c r="W4" s="31">
-        <v>0</v>
-      </c>
-      <c r="X4" s="31">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="31">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="31">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="31">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="31">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="34">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="31">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="31">
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0</v>
+      </c>
+      <c r="F4" s="30">
+        <v>0</v>
+      </c>
+      <c r="G4" s="30">
+        <v>0</v>
+      </c>
+      <c r="H4" s="30">
+        <v>0</v>
+      </c>
+      <c r="I4" s="30">
+        <v>0</v>
+      </c>
+      <c r="J4" s="30">
+        <v>0</v>
+      </c>
+      <c r="K4" s="30">
+        <v>0</v>
+      </c>
+      <c r="L4" s="30">
+        <v>0</v>
+      </c>
+      <c r="M4" s="30">
+        <v>0</v>
+      </c>
+      <c r="N4" s="30">
+        <v>0</v>
+      </c>
+      <c r="O4" s="30">
+        <v>0</v>
+      </c>
+      <c r="P4" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="30">
+        <v>0</v>
+      </c>
+      <c r="R4" s="30">
+        <v>0</v>
+      </c>
+      <c r="S4" s="16">
+        <v>0</v>
+      </c>
+      <c r="T4" s="16">
+        <v>0</v>
+      </c>
+      <c r="U4" s="16">
+        <v>0</v>
+      </c>
+      <c r="V4" s="16">
+        <v>0</v>
+      </c>
+      <c r="W4" s="30">
+        <v>0</v>
+      </c>
+      <c r="X4" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="33">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="33">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="33">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="33">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="33">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="33">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="16">
         <v>2</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>86.6</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>-50</v>
       </c>
-      <c r="E5" s="24">
-        <v>0</v>
-      </c>
-      <c r="F5" s="31">
-        <v>0</v>
-      </c>
-      <c r="G5" s="31">
-        <v>0</v>
-      </c>
-      <c r="H5" s="31">
-        <v>0</v>
-      </c>
-      <c r="I5" s="31">
-        <v>0</v>
-      </c>
-      <c r="J5" s="31">
-        <v>0</v>
-      </c>
-      <c r="K5" s="31">
-        <v>0</v>
-      </c>
-      <c r="L5" s="31">
-        <v>0</v>
-      </c>
-      <c r="M5" s="31">
-        <v>0</v>
-      </c>
-      <c r="N5" s="31">
-        <v>0</v>
-      </c>
-      <c r="O5" s="31">
-        <v>0</v>
-      </c>
-      <c r="P5" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="31">
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+      <c r="F5" s="30">
+        <v>0</v>
+      </c>
+      <c r="G5" s="30">
+        <v>0</v>
+      </c>
+      <c r="H5" s="30">
+        <v>0</v>
+      </c>
+      <c r="I5" s="30">
+        <v>0</v>
+      </c>
+      <c r="J5" s="30">
+        <v>0</v>
+      </c>
+      <c r="K5" s="30">
+        <v>0</v>
+      </c>
+      <c r="L5" s="30">
+        <v>0</v>
+      </c>
+      <c r="M5" s="30">
+        <v>0</v>
+      </c>
+      <c r="N5" s="30">
+        <v>0</v>
+      </c>
+      <c r="O5" s="30">
+        <v>0</v>
+      </c>
+      <c r="P5" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="30">
         <v>1</v>
       </c>
-      <c r="R5" s="31">
+      <c r="R5" s="30">
         <v>-0.52359999999999995</v>
       </c>
-      <c r="S5" s="17">
+      <c r="S5" s="16">
         <v>0.33610000000000001</v>
       </c>
-      <c r="T5" s="17">
+      <c r="T5" s="16">
         <v>13.79</v>
       </c>
-      <c r="U5" s="17">
+      <c r="U5" s="16">
         <v>1304.74</v>
       </c>
-      <c r="V5" s="17">
+      <c r="V5" s="16">
         <v>1312.9336000000001</v>
       </c>
-      <c r="W5" s="31">
-        <v>0</v>
-      </c>
-      <c r="X5" s="31">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="31">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="31">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="31">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="31">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="34">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="34">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="34">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="34">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="34">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="34">
+      <c r="W5" s="30">
+        <v>0</v>
+      </c>
+      <c r="X5" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="33">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="33">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="33">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="33">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="33">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="33">
         <v>5</v>
       </c>
-      <c r="AI5" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="31">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="31">
+      <c r="AI5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>3</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>418.1</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>-50</v>
       </c>
-      <c r="E6" s="24">
-        <v>0</v>
-      </c>
-      <c r="F6" s="31">
-        <v>0</v>
-      </c>
-      <c r="G6" s="31">
-        <v>0</v>
-      </c>
-      <c r="H6" s="31">
-        <v>0</v>
-      </c>
-      <c r="I6" s="31">
-        <v>0</v>
-      </c>
-      <c r="J6" s="31">
-        <v>0</v>
-      </c>
-      <c r="K6" s="31">
-        <v>0</v>
-      </c>
-      <c r="L6" s="31">
-        <v>0</v>
-      </c>
-      <c r="M6" s="31">
-        <v>0</v>
-      </c>
-      <c r="N6" s="31">
-        <v>0</v>
-      </c>
-      <c r="O6" s="31">
-        <v>0</v>
-      </c>
-      <c r="P6" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="31">
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+      <c r="F6" s="30">
+        <v>0</v>
+      </c>
+      <c r="G6" s="30">
+        <v>0</v>
+      </c>
+      <c r="H6" s="30">
+        <v>0</v>
+      </c>
+      <c r="I6" s="30">
+        <v>0</v>
+      </c>
+      <c r="J6" s="30">
+        <v>0</v>
+      </c>
+      <c r="K6" s="30">
+        <v>0</v>
+      </c>
+      <c r="L6" s="30">
+        <v>0</v>
+      </c>
+      <c r="M6" s="30">
+        <v>0</v>
+      </c>
+      <c r="N6" s="30">
+        <v>0</v>
+      </c>
+      <c r="O6" s="30">
+        <v>0</v>
+      </c>
+      <c r="P6" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="30">
         <v>1</v>
       </c>
-      <c r="R6" s="31">
+      <c r="R6" s="30">
         <v>0.20100000000000001</v>
       </c>
-      <c r="S6" s="17">
+      <c r="S6" s="16">
         <v>5.2492999999999999</v>
       </c>
-      <c r="T6" s="17">
+      <c r="T6" s="16">
         <v>1345.9128000000001</v>
       </c>
-      <c r="U6" s="17">
+      <c r="U6" s="16">
         <f>1.27307*10^5</f>
         <v>127306.99999999999</v>
       </c>
-      <c r="V6" s="32">
+      <c r="V6" s="31">
         <f>1.2810726*10^5</f>
         <v>128107.26</v>
       </c>
-      <c r="W6" s="31">
-        <v>0</v>
-      </c>
-      <c r="X6" s="31">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="31">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="31">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="31">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="31">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="31">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="31">
+      <c r="W6" s="30">
+        <v>0</v>
+      </c>
+      <c r="X6" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="33">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="33">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="33">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="33">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="33">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="33">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>4</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <v>720</v>
       </c>
-      <c r="D7" s="17">
-        <v>0</v>
-      </c>
-      <c r="E7" s="17">
-        <v>0</v>
-      </c>
-      <c r="F7" s="31">
-        <v>0</v>
-      </c>
-      <c r="G7" s="31">
-        <v>0</v>
-      </c>
-      <c r="H7" s="31">
-        <v>0</v>
-      </c>
-      <c r="I7" s="31">
-        <v>0</v>
-      </c>
-      <c r="J7" s="31">
-        <v>0</v>
-      </c>
-      <c r="K7" s="31">
-        <v>0</v>
-      </c>
-      <c r="L7" s="31">
-        <v>0</v>
-      </c>
-      <c r="M7" s="31">
-        <v>0</v>
-      </c>
-      <c r="N7" s="31">
-        <v>0</v>
-      </c>
-      <c r="O7" s="31">
-        <v>0</v>
-      </c>
-      <c r="P7" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="31">
-        <v>0</v>
-      </c>
-      <c r="R7" s="31">
-        <v>0</v>
-      </c>
-      <c r="S7" s="17">
+      <c r="D7" s="16">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0</v>
+      </c>
+      <c r="F7" s="30">
+        <v>0</v>
+      </c>
+      <c r="G7" s="30">
+        <v>0</v>
+      </c>
+      <c r="H7" s="30">
+        <v>0</v>
+      </c>
+      <c r="I7" s="30">
+        <v>0</v>
+      </c>
+      <c r="J7" s="30">
+        <v>0</v>
+      </c>
+      <c r="K7" s="30">
+        <v>0</v>
+      </c>
+      <c r="L7" s="30">
+        <v>0</v>
+      </c>
+      <c r="M7" s="30">
+        <v>0</v>
+      </c>
+      <c r="N7" s="30">
+        <v>0</v>
+      </c>
+      <c r="O7" s="30">
+        <v>0</v>
+      </c>
+      <c r="P7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>0</v>
+      </c>
+      <c r="R7" s="30">
+        <v>0</v>
+      </c>
+      <c r="S7" s="16">
         <v>2.9956</v>
       </c>
-      <c r="T7" s="17">
+      <c r="T7" s="16">
         <v>1997.056</v>
       </c>
-      <c r="U7" s="17">
+      <c r="U7" s="16">
         <v>3994.1</v>
       </c>
-      <c r="V7" s="17">
+      <c r="V7" s="16">
         <v>5192.3455999999996</v>
       </c>
-      <c r="W7" s="31">
-        <v>0</v>
-      </c>
-      <c r="X7" s="31">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="31">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="31">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="31">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="31">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="34">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="34">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="34">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="34">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="34">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="34">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="31">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="31">
+      <c r="W7" s="30">
+        <v>0</v>
+      </c>
+      <c r="X7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="33">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="33">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="33">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="33">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="33">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="33">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="30">
         <v>0</v>
       </c>
     </row>
@@ -3098,7 +3233,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="14"/>
+      <c r="O21" s="13"/>
       <c r="P21" s="3"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -3116,7 +3251,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="14"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -3134,7 +3269,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="14"/>
+      <c r="O23" s="13"/>
       <c r="P23" s="3"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -3152,7 +3287,7 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="14"/>
+      <c r="O24" s="13"/>
       <c r="P24" s="3"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -3170,7 +3305,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="14"/>
+      <c r="O25" s="13"/>
       <c r="P25" s="3"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -3188,7 +3323,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="14"/>
+      <c r="O26" s="13"/>
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -3206,7 +3341,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="14"/>
+      <c r="O27" s="13"/>
       <c r="P27" s="3"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -3224,7 +3359,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="14"/>
+      <c r="O28" s="13"/>
       <c r="P28" s="3"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -5979,16 +6114,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -6004,26 +6139,26 @@
       <c r="X1" s="10"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -6063,9 +6198,9 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
@@ -6083,9 +6218,9 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
@@ -6095,19 +6230,19 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -6117,34 +6252,34 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="82" t="s">
+      <c r="F6" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="83"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="82" t="s">
+      <c r="G6" s="82"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="J6" s="83"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
@@ -6154,14 +6289,14 @@
       <c r="X6" s="10"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -6177,22 +6312,22 @@
       <c r="X7" s="10"/>
     </row>
     <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="77"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="76"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -6217,21 +6352,21 @@
       <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="78" t="s">
+      <c r="F9" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="76" t="s">
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76" t="s">
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -6241,46 +6376,46 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="18">
         <v>4</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>3</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>4</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>663</v>
       </c>
-      <c r="G10" s="14">
-        <v>0</v>
-      </c>
-      <c r="H10" s="14">
-        <v>0</v>
-      </c>
-      <c r="I10" s="19">
+      <c r="G10" s="13">
+        <v>0</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="18">
         <v>663</v>
       </c>
-      <c r="J10" s="19">
-        <v>0</v>
-      </c>
-      <c r="K10" s="19">
+      <c r="J10" s="18">
+        <v>0</v>
+      </c>
+      <c r="K10" s="18">
         <v>1</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="20">
         <v>663</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="20">
         <v>1</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="20">
         <v>0</v>
       </c>
       <c r="R10" s="10"/>
@@ -6313,19 +6448,19 @@
       <c r="X11" s="10"/>
     </row>
     <row r="12" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
-      <c r="K12" s="77"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
@@ -6335,7 +6470,7 @@
       <c r="X12" s="10"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -6350,16 +6485,16 @@
       <c r="E13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="78" t="s">
+      <c r="F13" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="76" t="s">
+      <c r="G13" s="77"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="76"/>
-      <c r="K13" s="76"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -6369,37 +6504,37 @@
       <c r="X13" s="10"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="A14" s="13">
         <v>2</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>1</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <v>2</v>
       </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="14">
-        <v>0</v>
-      </c>
-      <c r="K14" s="14">
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
         <v>1</v>
       </c>
       <c r="R14" s="10"/>
@@ -6410,24 +6545,24 @@
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
+    <row r="15" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
@@ -6437,19 +6572,19 @@
       <c r="X16" s="10"/>
     </row>
     <row r="17" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="77"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="77"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="76"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
@@ -6459,44 +6594,44 @@
       <c r="X17" s="10"/>
     </row>
     <row r="18" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="78" t="s">
+      <c r="F18" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="76" t="s">
+      <c r="G18" s="77"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="76"/>
-      <c r="K18" s="76"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="75"/>
     </row>
     <row r="19" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
@@ -6520,19 +6655,19 @@
       <c r="X20" s="10"/>
     </row>
     <row r="21" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="77"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
@@ -6542,207 +6677,207 @@
       <c r="X21" s="10"/>
     </row>
     <row r="22" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="78" t="s">
+      <c r="F22" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="76" t="s">
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="76"/>
-      <c r="K22" s="76"/>
-    </row>
-    <row r="23" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
+      <c r="J22" s="75"/>
+      <c r="K22" s="75"/>
+    </row>
+    <row r="23" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
         <v>5</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="18">
         <v>4</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="18">
         <v>1</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="18">
         <v>660</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="18">
         <v>-40</v>
       </c>
-      <c r="H23" s="19">
-        <v>0</v>
-      </c>
-      <c r="I23" s="19">
+      <c r="H23" s="18">
+        <v>0</v>
+      </c>
+      <c r="I23" s="18">
         <v>1</v>
       </c>
-      <c r="J23" s="19">
-        <v>0</v>
-      </c>
-      <c r="K23" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:24" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="77" t="s">
+      <c r="J23" s="18">
+        <v>0</v>
+      </c>
+      <c r="K23" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="76" t="s">
         <v>136</v>
       </c>
-      <c r="B25" s="77"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="77"/>
-      <c r="N25" s="77"/>
-    </row>
-    <row r="26" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="B25" s="76"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
+      <c r="M25" s="76"/>
+      <c r="N25" s="76"/>
+    </row>
+    <row r="26" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="38" t="s">
+      <c r="E26" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="78" t="s">
+      <c r="F26" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="76" t="s">
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="J26" s="76"/>
-      <c r="K26" s="76"/>
-      <c r="L26" s="76" t="s">
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="M26" s="76"/>
-      <c r="N26" s="76"/>
-    </row>
-    <row r="27" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:24" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="77" t="s">
+      <c r="M26" s="75"/>
+      <c r="N26" s="75"/>
+    </row>
+    <row r="27" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="76" t="s">
         <v>138</v>
       </c>
-      <c r="B29" s="77"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="77"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="77"/>
-      <c r="G29" s="77"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="77"/>
-      <c r="J29" s="77"/>
-      <c r="K29" s="77"/>
-      <c r="L29" s="77"/>
-      <c r="M29" s="77"/>
-      <c r="N29" s="77"/>
-      <c r="O29" s="77"/>
-      <c r="P29" s="77"/>
-      <c r="Q29" s="77"/>
-    </row>
-    <row r="30" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="76"/>
+      <c r="I29" s="76"/>
+      <c r="J29" s="76"/>
+      <c r="K29" s="76"/>
+      <c r="L29" s="76"/>
+      <c r="M29" s="76"/>
+      <c r="N29" s="76"/>
+      <c r="O29" s="76"/>
+      <c r="P29" s="76"/>
+      <c r="Q29" s="76"/>
+    </row>
+    <row r="30" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="38" t="s">
+      <c r="C30" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D30" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="38" t="s">
+      <c r="E30" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="82" t="s">
+      <c r="F30" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="G30" s="83"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="82" t="s">
+      <c r="G30" s="82"/>
+      <c r="H30" s="83"/>
+      <c r="I30" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="J30" s="83"/>
-      <c r="K30" s="84"/>
-      <c r="L30" s="76" t="s">
+      <c r="J30" s="82"/>
+      <c r="K30" s="83"/>
+      <c r="L30" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="M30" s="76"/>
-      <c r="N30" s="76"/>
-      <c r="O30" s="76" t="s">
+      <c r="M30" s="75"/>
+      <c r="N30" s="75"/>
+      <c r="O30" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="P30" s="76"/>
-      <c r="Q30" s="76"/>
-    </row>
-    <row r="31" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="21"/>
+      <c r="P30" s="75"/>
+      <c r="Q30" s="75"/>
+    </row>
+    <row r="31" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
     </row>
     <row r="32" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="77" t="s">
+      <c r="A33" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="77"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
@@ -6757,22 +6892,22 @@
       <c r="X33" s="10"/>
     </row>
     <row r="34" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="15" t="s">
         <v>18</v>
       </c>
       <c r="G34" s="12"/>
@@ -6782,12 +6917,12 @@
       <c r="K34" s="12"/>
     </row>
     <row r="35" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
@@ -6816,12 +6951,12 @@
       <c r="X36" s="10"/>
     </row>
     <row r="37" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="77" t="s">
+      <c r="A37" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="77"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
+      <c r="B37" s="76"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
@@ -6838,7 +6973,7 @@
       <c r="X37" s="10"/>
     </row>
     <row r="38" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B38" s="8" t="s">
@@ -6893,15 +7028,15 @@
       <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="79" t="s">
+      <c r="A41" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="80"/>
-      <c r="C41" s="80"/>
-      <c r="D41" s="80"/>
-      <c r="E41" s="80"/>
-      <c r="F41" s="80"/>
-      <c r="G41" s="81"/>
+      <c r="B41" s="79"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="79"/>
+      <c r="F41" s="79"/>
+      <c r="G41" s="80"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
       <c r="J41" s="10"/>
@@ -6909,7 +7044,7 @@
       <c r="L41" s="9"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -6921,87 +7056,87 @@
       <c r="D42" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="76" t="s">
+      <c r="E42" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="F42" s="76"/>
-      <c r="G42" s="76"/>
+      <c r="F42" s="75"/>
+      <c r="G42" s="75"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
     <row r="43" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14">
+      <c r="A43" s="13">
         <v>1</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="14">
+      <c r="D43" s="13">
         <v>1</v>
       </c>
-      <c r="E43" s="14">
-        <v>0</v>
-      </c>
-      <c r="F43" s="14">
-        <v>0</v>
-      </c>
-      <c r="G43" s="14">
+      <c r="E43" s="13">
+        <v>0</v>
+      </c>
+      <c r="F43" s="13">
+        <v>0</v>
+      </c>
+      <c r="G43" s="13">
         <v>0</v>
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
     </row>
     <row r="44" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14">
+      <c r="A44" s="13">
         <v>2</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="13">
         <v>2</v>
       </c>
-      <c r="E44" s="14">
+      <c r="E44" s="13">
         <v>173.2</v>
       </c>
-      <c r="F44" s="14">
+      <c r="F44" s="13">
         <f>-100</f>
         <v>-100</v>
       </c>
-      <c r="G44" s="14">
+      <c r="G44" s="13">
         <v>0</v>
       </c>
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
     </row>
     <row r="45" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="14">
+      <c r="A45" s="13">
         <v>3</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D45" s="13">
         <v>3</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45" s="13">
         <v>663</v>
       </c>
-      <c r="F45" s="14">
-        <v>0</v>
-      </c>
-      <c r="G45" s="14">
+      <c r="F45" s="13">
+        <v>0</v>
+      </c>
+      <c r="G45" s="13">
         <v>0</v>
       </c>
       <c r="H45"/>
@@ -7010,25 +7145,25 @@
       <c r="K45" s="12"/>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A46" s="14">
+      <c r="A46" s="13">
         <v>4</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D46" s="13">
         <v>4</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E46" s="13">
         <v>763</v>
       </c>
-      <c r="F46" s="14">
-        <v>0</v>
-      </c>
-      <c r="G46" s="14">
+      <c r="F46" s="13">
+        <v>0</v>
+      </c>
+      <c r="G46" s="13">
         <v>0</v>
       </c>
     </row>
@@ -7038,13 +7173,13 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
     </row>
     <row r="64" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -7115,61 +7250,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="86"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="26" t="s">
+      <c r="G2" s="85"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="27" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="14"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I4" s="27"/>
+      <c r="I4" s="26"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
@@ -7195,7 +7330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F55610B-D925-4735-AE3D-EBBD0AD81ACC}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
@@ -7218,503 +7353,503 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="95" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
     </row>
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="102" t="s">
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="101" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="104"/>
-      <c r="U2" s="90" t="s">
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="103"/>
+      <c r="U2" s="89" t="s">
         <v>132</v>
       </c>
-      <c r="V2" s="90"/>
-      <c r="W2" s="90"/>
-      <c r="X2" s="90"/>
-      <c r="Y2" s="90"/>
-      <c r="Z2" s="90"/>
+      <c r="V2" s="89"/>
+      <c r="W2" s="89"/>
+      <c r="X2" s="89"/>
+      <c r="Y2" s="89"/>
+      <c r="Z2" s="89"/>
     </row>
     <row r="3" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="92"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="94" t="s">
+      <c r="G3" s="91"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="41" t="s">
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="M3" s="35" t="s">
+      <c r="M3" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="N3" s="35" t="s">
+      <c r="N3" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="O3" s="35" t="s">
+      <c r="O3" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="P3" s="41" t="s">
+      <c r="P3" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="Q3" s="95" t="s">
+      <c r="Q3" s="94" t="s">
         <v>131</v>
       </c>
-      <c r="R3" s="95"/>
-      <c r="U3" s="90"/>
-      <c r="V3" s="90"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="90"/>
-      <c r="Y3" s="90"/>
-      <c r="Z3" s="90"/>
+      <c r="R3" s="94"/>
+      <c r="U3" s="89"/>
+      <c r="V3" s="89"/>
+      <c r="W3" s="89"/>
+      <c r="X3" s="89"/>
+      <c r="Y3" s="89"/>
+      <c r="Z3" s="89"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="90"/>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="89"/>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="L5" s="19"/>
-      <c r="U5" s="90"/>
-      <c r="V5" s="90"/>
-      <c r="W5" s="90"/>
-      <c r="X5" s="90"/>
-      <c r="Y5" s="90"/>
-      <c r="Z5" s="90"/>
+      <c r="L5" s="18"/>
+      <c r="U5" s="89"/>
+      <c r="V5" s="89"/>
+      <c r="W5" s="89"/>
+      <c r="X5" s="89"/>
+      <c r="Y5" s="89"/>
+      <c r="Z5" s="89"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U6" s="90"/>
-      <c r="V6" s="90"/>
-      <c r="W6" s="90"/>
-      <c r="X6" s="90"/>
-      <c r="Y6" s="90"/>
-      <c r="Z6" s="90"/>
+      <c r="U6" s="89"/>
+      <c r="V6" s="89"/>
+      <c r="W6" s="89"/>
+      <c r="X6" s="89"/>
+      <c r="Y6" s="89"/>
+      <c r="Z6" s="89"/>
     </row>
     <row r="7" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="97"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="97"/>
-      <c r="H7" s="97"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="97"/>
-      <c r="K7" s="97"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="97"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="97"/>
-      <c r="P7" s="97"/>
-      <c r="Q7" s="97"/>
-      <c r="R7" s="97"/>
-      <c r="U7" s="90"/>
-      <c r="V7" s="90"/>
-      <c r="W7" s="90"/>
-      <c r="X7" s="90"/>
-      <c r="Y7" s="90"/>
-      <c r="Z7" s="90"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="96"/>
+      <c r="O7" s="96"/>
+      <c r="P7" s="96"/>
+      <c r="Q7" s="96"/>
+      <c r="R7" s="96"/>
+      <c r="U7" s="89"/>
+      <c r="V7" s="89"/>
+      <c r="W7" s="89"/>
+      <c r="X7" s="89"/>
+      <c r="Y7" s="89"/>
+      <c r="Z7" s="89"/>
     </row>
     <row r="8" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="77"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="98" t="s">
+      <c r="A8" s="76"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="97" t="s">
         <v>128</v>
       </c>
-      <c r="N8" s="99"/>
-      <c r="O8" s="99"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="99"/>
-      <c r="R8" s="100"/>
-      <c r="U8" s="90"/>
-      <c r="V8" s="90"/>
-      <c r="W8" s="90"/>
-      <c r="X8" s="90"/>
-      <c r="Y8" s="90"/>
-      <c r="Z8" s="90"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="98"/>
+      <c r="P8" s="98"/>
+      <c r="Q8" s="98"/>
+      <c r="R8" s="99"/>
+      <c r="U8" s="89"/>
+      <c r="V8" s="89"/>
+      <c r="W8" s="89"/>
+      <c r="X8" s="89"/>
+      <c r="Y8" s="89"/>
+      <c r="Z8" s="89"/>
     </row>
     <row r="9" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="91" t="s">
+      <c r="F9" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="92"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="94" t="s">
+      <c r="G9" s="91"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="41" t="s">
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="M9" s="43" t="s">
+      <c r="M9" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="N9" s="43" t="s">
+      <c r="N9" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="O9" s="43" t="s">
+      <c r="O9" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="P9" s="44" t="s">
+      <c r="P9" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="Q9" s="91" t="s">
+      <c r="Q9" s="90" t="s">
         <v>130</v>
       </c>
-      <c r="R9" s="93"/>
-      <c r="U9" s="90"/>
-      <c r="V9" s="90"/>
-      <c r="W9" s="90"/>
-      <c r="X9" s="90"/>
-      <c r="Y9" s="90"/>
-      <c r="Z9" s="90"/>
+      <c r="R9" s="92"/>
+      <c r="U9" s="89"/>
+      <c r="V9" s="89"/>
+      <c r="W9" s="89"/>
+      <c r="X9" s="89"/>
+      <c r="Y9" s="89"/>
+      <c r="Z9" s="89"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="27"/>
-      <c r="U10" s="90"/>
-      <c r="V10" s="90"/>
-      <c r="W10" s="90"/>
-      <c r="X10" s="90"/>
-      <c r="Y10" s="90"/>
-      <c r="Z10" s="90"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="26"/>
+      <c r="U10" s="89"/>
+      <c r="V10" s="89"/>
+      <c r="W10" s="89"/>
+      <c r="X10" s="89"/>
+      <c r="Y10" s="89"/>
+      <c r="Z10" s="89"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="U11" s="90"/>
-      <c r="V11" s="90"/>
-      <c r="W11" s="90"/>
-      <c r="X11" s="90"/>
-      <c r="Y11" s="90"/>
-      <c r="Z11" s="90"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="U11" s="89"/>
+      <c r="V11" s="89"/>
+      <c r="W11" s="89"/>
+      <c r="X11" s="89"/>
+      <c r="Y11" s="89"/>
+      <c r="Z11" s="89"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U12" s="90"/>
-      <c r="V12" s="90"/>
-      <c r="W12" s="90"/>
-      <c r="X12" s="90"/>
-      <c r="Y12" s="90"/>
-      <c r="Z12" s="90"/>
+      <c r="U12" s="89"/>
+      <c r="V12" s="89"/>
+      <c r="W12" s="89"/>
+      <c r="X12" s="89"/>
+      <c r="Y12" s="89"/>
+      <c r="Z12" s="89"/>
     </row>
     <row r="13" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="80"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="U13" s="90"/>
-      <c r="V13" s="90"/>
-      <c r="W13" s="90"/>
-      <c r="X13" s="90"/>
-      <c r="Y13" s="90"/>
-      <c r="Z13" s="90"/>
-    </row>
-    <row r="14" spans="1:26" s="36" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
+      <c r="N13" s="79"/>
+      <c r="O13" s="79"/>
+      <c r="P13" s="79"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+      <c r="U13" s="89"/>
+      <c r="V13" s="89"/>
+      <c r="W13" s="89"/>
+      <c r="X13" s="89"/>
+      <c r="Y13" s="89"/>
+      <c r="Z13" s="89"/>
+    </row>
+    <row r="14" spans="1:26" s="35" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="94" t="s">
+      <c r="F14" s="93" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="41" t="s">
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="101" t="s">
+      <c r="J14" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="101"/>
-      <c r="L14" s="101"/>
-      <c r="M14" s="101" t="s">
+      <c r="K14" s="100"/>
+      <c r="L14" s="100"/>
+      <c r="M14" s="100" t="s">
         <v>84</v>
       </c>
-      <c r="N14" s="101"/>
-      <c r="O14" s="101"/>
-      <c r="P14" s="37" t="s">
+      <c r="N14" s="100"/>
+      <c r="O14" s="100"/>
+      <c r="P14" s="36" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="39"/>
-      <c r="S15" s="39"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="38"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="38"/>
     </row>
     <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="78" t="s">
         <v>162</v>
       </c>
-      <c r="B17" s="80"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="80"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="49" t="s">
+      <c r="E18" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54" t="s">
         <v>171</v>
       </c>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="34" t="s">
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="33" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -7748,82 +7883,42 @@
   <dimension ref="A2:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q11" sqref="G11:Q11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="104" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="105"/>
+      <c r="B2" s="104"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G9" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40">
-        <v>2</v>
-      </c>
-      <c r="J9" s="40">
-        <v>4</v>
-      </c>
-      <c r="K9" s="40">
-        <v>0</v>
-      </c>
-      <c r="L9" s="40">
-        <v>0</v>
-      </c>
-      <c r="M9" s="40">
-        <v>0</v>
-      </c>
-      <c r="N9" s="40">
-        <v>663</v>
-      </c>
-      <c r="O9" s="40">
-        <v>0</v>
-      </c>
-      <c r="P9" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="19">
-        <v>1</v>
-      </c>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="18"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G11" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40">
-        <v>2</v>
-      </c>
-      <c r="J11" s="40">
-        <v>4</v>
-      </c>
-      <c r="K11" s="40">
-        <v>0</v>
-      </c>
-      <c r="L11" s="40">
-        <v>0</v>
-      </c>
-      <c r="M11" s="40">
-        <v>0</v>
-      </c>
-      <c r="N11" s="40">
-        <v>663</v>
-      </c>
-      <c r="O11" s="40">
-        <v>0</v>
-      </c>
-      <c r="P11" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="40">
-        <v>0.5</v>
-      </c>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>